<commit_message>
added huson and alita talk desc.
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\public works\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3734AF-A0DF-4ED5-B937-75E9B1E4C2AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE7C9E3-74F6-460D-89A9-E6F14A45F7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
+    <workbookView xWindow="7200" yWindow="1725" windowWidth="21600" windowHeight="11385" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -365,9 +365,6 @@
     <t>Alita Howard</t>
   </si>
   <si>
-    <t>Dr. Heather Huson and Dr. Srikanth Krisnamoorthy</t>
-  </si>
-  <si>
     <t>Cornell Dept. of Animal Science</t>
   </si>
   <si>
@@ -380,22 +377,25 @@
     <t>Chess on Ice: The Science, Strategy, and History of Curling</t>
   </si>
   <si>
-    <t>Balto, Elite Sled Dog and Hero of the 1925 Serum Run to Nome, Alaska: A story of a dog through his genome</t>
-  </si>
-  <si>
-    <t>Details coming soon!</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Details coming soon, but here's a photo of Dr. Huson racing as a musher in Alaska!&lt;div class="box"&gt; &lt;img src="images/huson_sled.jpg" style = 'width: 550' class='center'&gt; &lt;/div&gt;</t>
-  </si>
-  <si>
     <t>With a global population approaching 10 billion people, how can we bring Earth’s population to the living standards of the United States and/or the European Union while simultaneously reducing greenhouse gas emissions? In this talk, Dr. Hawkins will introduce the audience to the nuanced challenge of simultaneously tackling climate change while expanding access to energy infrastructure in under-developed regions of the world. Topics will include limitations of intermittent electricity suppliers, options for baseload power generators, and the potential of geothermal energy to transform global energy infrastructure, including the Earth Source Heat project at Cornell University.&lt;br&gt;&lt;br&gt;&lt;div class="box"&gt;  &lt;img src="images/hawkinsbanner.jpg" class='center'&gt; &lt;/div&gt;</t>
   </si>
   <si>
     <t>In 2024 the Europa Clipper will launch on a SpaceX Falcon Heavy rocket to begin its five and half year trip to Jupiter, where it will study the icy ocean world of Europa (which is one of the best bets for alien life in our own solar system!). But for quite some time, NASA mission planners had to allow for the possibility of launching on both the Falcon Heavy and the United Launch Alliance Space Launch System (SLS). Why? Because the SLS had friends in congress, of course. In this talk, we'll learn about how congressional politics can make life hell for mission planning, why NASA missions are so expensive, what single points of failure are, and why the indecision of launch vehicles can burn unbelievable sums of money. We'll also look at the Galileo spacecraft as a cautionary tale about changing mission parameters late in the game.&lt;br&gt;&lt;br&gt;&lt;div class="box"&gt;  &lt;img src="images/ulibarri.png" style = 'width: 550' class='center'&gt; &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Finger Lakes Curling Board Member</t>
+  </si>
+  <si>
+    <t>Dr. Heather Huson and Dr. Srikanth Krishnamoorthy</t>
+  </si>
+  <si>
+    <t>The Story of Balto, an Elite Sled Dog: Through his Genome</t>
+  </si>
+  <si>
+    <t>Almost 100 years ago, Balto, along with a pack of elite sled dogs helped save the community of Nome, Alaska, from a diphtheria outbreak. Balto is representative of the sled dogs of the era who were reputed for their hardiness, endurance, and tolerance of harsh conditions at a time when northern communities relied on them for transportation, protection, and companionship. Unlike modern breeds, Balto and his contemporaries were products of generations of mating of diverse, outbred dogs selected for their performance and hardiness.  Today, Balto is immortalized with a statue in Central Park and is physically preserved and on display at the Cleaveland Museum of Natural History. We asked ourselves, could we use advances in genomic technologies and ancient DNA recovery techniques to parse through Balto’s DNA and understand selection emphasis and diversity occurring in sled dogs in the 1930’s? Could we decipher Balto’s physical appearance from his DNA and identify healthy developmental gene variants that may have endowed sled dogs in that era with abilities to withstand and thrive in harsh environments? Could we use our findings to guide modern breeders to breed healthier dogs? &lt;br&gt;&lt;br&gt;Also, here's a photo of Dr. Huson racing as a musher in Alaska!&lt;div class="box"&gt; &lt;img src="images/huson_sled.jpg" style = 'width: 550' class='center'&gt; &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have you seen curling on TV, that weird game with stones, and brooms, and people yelling at each other on ice?  Maybe you caught the fever back in 2018, watching the Men’s curling team win USA’s first gold medal in the sport, saw it in a movie, or have visited Canada at any point in your life.  Alita started curling with the Finger Lakes Curling Club in 2018 after taking one of the first Learn to Curl’s, soon after the club’s founding.  She currently skips, is an instructor, volunteers on the club’s board, and travels to friendlies and bonspiels to compete and meet other curlers.  In a Public Works’ version of broomstacking, Alita will talk about the history, explain the types and rules of curling, and delve a little into the science, all while taking part in a major part of curling: drinking beverages. </t>
   </si>
 </sst>
 </file>
@@ -750,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F859F76-284E-4154-B5CC-2AAD28AB7940}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1221,7 +1221,7 @@
         <v>92</v>
       </c>
       <c r="H18" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1247,7 +1247,7 @@
         <v>93</v>
       </c>
       <c r="H19" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1313,19 +1313,19 @@
         <v>2023</v>
       </c>
       <c r="D22" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="F22" t="s">
         <v>111</v>
       </c>
       <c r="G22" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="H22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1339,22 +1339,23 @@
         <v>2023</v>
       </c>
       <c r="D23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F23" t="s">
         <v>110</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>112</v>
       </c>
-      <c r="G23" t="s">
-        <v>114</v>
-      </c>
       <c r="H23" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added FarmNet and Ithaca Voice
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\public works\ithacapublicworks.github.io\generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE7C9E3-74F6-460D-89A9-E6F14A45F7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09955A5-1C5F-4C64-88DB-D8B6E236C0FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="1725" windowWidth="21600" windowHeight="11385" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
+    <workbookView xWindow="10" yWindow="0" windowWidth="19180" windowHeight="10080" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="131">
   <si>
     <t>speaker</t>
   </si>
@@ -396,6 +396,39 @@
   </si>
   <si>
     <t xml:space="preserve">Have you seen curling on TV, that weird game with stones, and brooms, and people yelling at each other on ice?  Maybe you caught the fever back in 2018, watching the Men’s curling team win USA’s first gold medal in the sport, saw it in a movie, or have visited Canada at any point in your life.  Alita started curling with the Finger Lakes Curling Club in 2018 after taking one of the first Learn to Curl’s, soon after the club’s founding.  She currently skips, is an instructor, volunteers on the club’s board, and travels to friendlies and bonspiels to compete and meet other curlers.  In a Public Works’ version of broomstacking, Alita will talk about the history, explain the types and rules of curling, and delve a little into the science, all while taking part in a major part of curling: drinking beverages. </t>
+  </si>
+  <si>
+    <t>October 4th</t>
+  </si>
+  <si>
+    <t>Adam Howell</t>
+  </si>
+  <si>
+    <t>Everyone is aware of the price of food – from kitchen tables to restaurant counters, food costs impact our lives in profound ways. But another, less understood cost associated with our food is born out of the pressures faced by farmers as they struggle to succeed working in one of the most unforgiving industries in America. Farmers deal with numerous stressors outside of their control including market pressures, weather, price increases, supplies, and many more. Furthermore, farmers deal with the geographic challenge of being isolated from support services in rural areas, and cultural/psychological challenges stemming from personal stigmas against seeking help.&lt;br&gt;&lt;br&gt;In this Public Works talk, learn about a unique program in NYS that provides free, confidential support for farmers to help with any number of issues they may face. NY FarmNet approaches farm assistance and support through a “holistic” model by deploying a consultant team representing both the personal and financial aspects of every challenge.</t>
+  </si>
+  <si>
+    <t>For Whom the Dinner Bell Tolls: The Struggles of America’s Farming Community and How NY FarmNet Helps</t>
+  </si>
+  <si>
+    <t>an agriculture</t>
+  </si>
+  <si>
+    <t>Outreach Director, FarmNet Cornell</t>
+  </si>
+  <si>
+    <t>Jimmy Jordan</t>
+  </si>
+  <si>
+    <t>Columnist at Ithaca Voice</t>
+  </si>
+  <si>
+    <t>a journalism</t>
+  </si>
+  <si>
+    <t>Where the Media Death Spiral Brought Us: The Decline of Local Reporting, and an Industry Looking for its Footing</t>
+  </si>
+  <si>
+    <t>Details coming soon!</t>
   </si>
 </sst>
 </file>
@@ -452,7 +485,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -748,15 +781,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F859F76-284E-4154-B5CC-2AAD28AB7940}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -782,7 +815,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -808,7 +841,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -834,7 +867,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -860,7 +893,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2</v>
       </c>
@@ -886,7 +919,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>3</v>
       </c>
@@ -912,7 +945,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>3</v>
       </c>
@@ -938,7 +971,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>4</v>
       </c>
@@ -964,7 +997,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>4</v>
       </c>
@@ -990,7 +1023,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>5</v>
       </c>
@@ -1016,7 +1049,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1042,7 +1075,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>6</v>
       </c>
@@ -1068,7 +1101,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1094,7 +1127,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1120,7 +1153,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>7</v>
       </c>
@@ -1146,7 +1179,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1172,7 +1205,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>8</v>
       </c>
@@ -1198,7 +1231,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>9</v>
       </c>
@@ -1224,7 +1257,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>9</v>
       </c>
@@ -1250,7 +1283,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>10</v>
       </c>
@@ -1276,7 +1309,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>10</v>
       </c>
@@ -1302,7 +1335,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>11</v>
       </c>
@@ -1328,7 +1361,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>11</v>
       </c>
@@ -1352,6 +1385,58 @@
       </c>
       <c r="H23" t="s">
         <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>120</v>
+      </c>
+      <c r="C24">
+        <v>2023</v>
+      </c>
+      <c r="D24" t="s">
+        <v>121</v>
+      </c>
+      <c r="E24" t="s">
+        <v>125</v>
+      </c>
+      <c r="F24" t="s">
+        <v>124</v>
+      </c>
+      <c r="G24" t="s">
+        <v>123</v>
+      </c>
+      <c r="H24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25">
+        <v>2023</v>
+      </c>
+      <c r="D25" t="s">
+        <v>126</v>
+      </c>
+      <c r="E25" t="s">
+        <v>127</v>
+      </c>
+      <c r="F25" t="s">
+        <v>128</v>
+      </c>
+      <c r="G25" t="s">
+        <v>129</v>
+      </c>
+      <c r="H25" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Jimmy Jordan Abstract
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09955A5-1C5F-4C64-88DB-D8B6E236C0FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AD3302-B203-4BA3-A34A-4669DD08DBD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10" yWindow="0" windowWidth="19180" windowHeight="10080" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
@@ -428,7 +428,7 @@
     <t>Where the Media Death Spiral Brought Us: The Decline of Local Reporting, and an Industry Looking for its Footing</t>
   </si>
   <si>
-    <t>Details coming soon!</t>
+    <t xml:space="preserve">The newspaper industry in the U.S. has been undergoing a significant decline since the early 2000s. The rise of the internet ushered in an era of information abundance and accessibility. However, this transition has severely impacted the traditional business models that once supported local newspapers, resulting in noticeable gaps in community coverage across the country. All of this is set against a climate where trust in media is approaching historic lows in the U.S.&lt;br&gt;&lt;br&gt;This presentation will illustrate these challenges, both on a local scale and within a broader context. Additionally, we will delve into the new models that are being explored in an effort to revitalize local reporting. </t>
   </si>
 </sst>
 </file>
@@ -783,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F859F76-284E-4154-B5CC-2AAD28AB7940}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1398,19 +1398,19 @@
         <v>2023</v>
       </c>
       <c r="D24" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="E24" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F24" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="G24" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="H24" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -1424,19 +1424,19 @@
         <v>2023</v>
       </c>
       <c r="D25" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F25" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G25" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="H25" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated Jimmy Jordan's abstract again
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AD3302-B203-4BA3-A34A-4669DD08DBD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30479D16-B9AF-4194-B60B-52645FF674EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10" yWindow="0" windowWidth="19180" windowHeight="10080" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
@@ -784,7 +784,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
fixed typo in ghostwriting
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39474DA9-6392-47B9-9316-34A4C4638A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FB780F-BA03-4DBE-9938-A37CDB59B5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10" yWindow="0" windowWidth="19180" windowHeight="10080" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
@@ -446,9 +446,6 @@
     <t>Writer and Brand Manager</t>
   </si>
   <si>
-    <t>a ghost writing</t>
-  </si>
-  <si>
     <t>a psychology</t>
   </si>
   <si>
@@ -456,6 +453,9 @@
   </si>
   <si>
     <t>Title coming soon!</t>
+  </si>
+  <si>
+    <t>a ghostwriting</t>
   </si>
 </sst>
 </file>
@@ -811,7 +811,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1483,13 +1483,13 @@
         <v>135</v>
       </c>
       <c r="F26" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="G26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -1509,13 +1509,13 @@
         <v>134</v>
       </c>
       <c r="F27" t="s">
+        <v>136</v>
+      </c>
+      <c r="G27" t="s">
+        <v>138</v>
+      </c>
+      <c r="H27" t="s">
         <v>137</v>
-      </c>
-      <c r="G27" t="s">
-        <v>139</v>
-      </c>
-      <c r="H27" t="s">
-        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated generator code to include hash
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\public works\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE7C9E3-74F6-460D-89A9-E6F14A45F7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D14E38-A584-4C75-8E9C-440C62B7A47A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="1725" windowWidth="21600" windowHeight="11385" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="143">
   <si>
     <t>speaker</t>
   </si>
@@ -392,10 +392,79 @@
     <t>The Story of Balto, an Elite Sled Dog: Through his Genome</t>
   </si>
   <si>
-    <t>Almost 100 years ago, Balto, along with a pack of elite sled dogs helped save the community of Nome, Alaska, from a diphtheria outbreak. Balto is representative of the sled dogs of the era who were reputed for their hardiness, endurance, and tolerance of harsh conditions at a time when northern communities relied on them for transportation, protection, and companionship. Unlike modern breeds, Balto and his contemporaries were products of generations of mating of diverse, outbred dogs selected for their performance and hardiness.  Today, Balto is immortalized with a statue in Central Park and is physically preserved and on display at the Cleaveland Museum of Natural History. We asked ourselves, could we use advances in genomic technologies and ancient DNA recovery techniques to parse through Balto’s DNA and understand selection emphasis and diversity occurring in sled dogs in the 1930’s? Could we decipher Balto’s physical appearance from his DNA and identify healthy developmental gene variants that may have endowed sled dogs in that era with abilities to withstand and thrive in harsh environments? Could we use our findings to guide modern breeders to breed healthier dogs? &lt;br&gt;&lt;br&gt;Also, here's a photo of Dr. Huson racing as a musher in Alaska!&lt;div class="box"&gt; &lt;img src="images/huson_sled.jpg" style = 'width: 550' class='center'&gt; &lt;/div&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">Have you seen curling on TV, that weird game with stones, and brooms, and people yelling at each other on ice?  Maybe you caught the fever back in 2018, watching the Men’s curling team win USA’s first gold medal in the sport, saw it in a movie, or have visited Canada at any point in your life.  Alita started curling with the Finger Lakes Curling Club in 2018 after taking one of the first Learn to Curl’s, soon after the club’s founding.  She currently skips, is an instructor, volunteers on the club’s board, and travels to friendlies and bonspiels to compete and meet other curlers.  In a Public Works’ version of broomstacking, Alita will talk about the history, explain the types and rules of curling, and delve a little into the science, all while taking part in a major part of curling: drinking beverages. </t>
+  </si>
+  <si>
+    <t>Almost 100 years ago, Balto, along with a pack of elite sled dogs helped save the community of Nome, Alaska, from a diphtheria outbreak. Balto is representative of the sled dogs of the era who were reputed for their hardiness, endurance, and tolerance of harsh conditions at a time when northern communities relied on them for transportation, protection, and companionship. Unlike modern breeds, Balto and his contemporaries were products of generations of mating of diverse, outbred dogs selected for their performance and hardiness.  Today, Balto is immortalized with a statue in Central Park and is physically preserved and on display at the Cleveland Museum of Natural History. We asked ourselves, could we use advances in genomic technologies and ancient DNA recovery techniques to parse through Balto’s DNA and understand selection emphasis and diversity occurring in sled dogs in the 1930’s? Could we decipher Balto’s physical appearance from his DNA and identify healthy developmental gene variants that may have endowed sled dogs in that era with abilities to withstand and thrive in harsh environments? Could we use our findings to guide modern breeders to breed healthier dogs? &lt;br&gt;&lt;br&gt;Also, here's a photo of Dr. Huson racing as a musher in Alaska!&lt;div class="box"&gt; &lt;img src="images/huson_sled.jpg" style = 'width: 550' class='center'&gt; &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>hashcode</t>
+  </si>
+  <si>
+    <t>sethkorproski</t>
+  </si>
+  <si>
+    <t>zachulibarri</t>
+  </si>
+  <si>
+    <t>evesnyder</t>
+  </si>
+  <si>
+    <t>jamesnagy</t>
+  </si>
+  <si>
+    <t>benfried</t>
+  </si>
+  <si>
+    <t>ligiacoelho</t>
+  </si>
+  <si>
+    <t>meganbarrington</t>
+  </si>
+  <si>
+    <t>sethstrickland</t>
+  </si>
+  <si>
+    <t>danielasamur</t>
+  </si>
+  <si>
+    <t>lukekeller</t>
+  </si>
+  <si>
+    <t>hunteradams</t>
+  </si>
+  <si>
+    <t>michaelcaporizzo</t>
+  </si>
+  <si>
+    <t>mollyryan</t>
+  </si>
+  <si>
+    <t>karlsmolenski</t>
+  </si>
+  <si>
+    <t>daisyrosas</t>
+  </si>
+  <si>
+    <t>alisonritterhaus</t>
+  </si>
+  <si>
+    <t>zachulibarri2</t>
+  </si>
+  <si>
+    <t>adamhawkins</t>
+  </si>
+  <si>
+    <t>jayleeming</t>
+  </si>
+  <si>
+    <t>danielsprocket</t>
+  </si>
+  <si>
+    <t>heatherhuson</t>
+  </si>
+  <si>
+    <t>alitahoward</t>
   </si>
 </sst>
 </file>
@@ -748,15 +817,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F859F76-284E-4154-B5CC-2AAD28AB7940}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -781,8 +856,11 @@
       <c r="H1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -807,8 +885,11 @@
       <c r="H2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -833,8 +914,11 @@
       <c r="H3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -859,8 +943,11 @@
       <c r="H4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -885,8 +972,11 @@
       <c r="H5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -911,8 +1001,11 @@
       <c r="H6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -937,8 +1030,11 @@
       <c r="H7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -963,8 +1059,11 @@
       <c r="H8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -989,8 +1088,11 @@
       <c r="H9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -1015,8 +1117,11 @@
       <c r="H10" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1041,8 +1146,11 @@
       <c r="H11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -1067,8 +1175,11 @@
       <c r="H12" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1093,8 +1204,11 @@
       <c r="H13" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1119,8 +1233,11 @@
       <c r="H14" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
@@ -1145,8 +1262,11 @@
       <c r="H15" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1171,8 +1291,11 @@
       <c r="H16" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>8</v>
       </c>
@@ -1197,8 +1320,11 @@
       <c r="H17" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>9</v>
       </c>
@@ -1223,8 +1349,11 @@
       <c r="H18" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>9</v>
       </c>
@@ -1249,8 +1378,11 @@
       <c r="H19" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>10</v>
       </c>
@@ -1275,8 +1407,11 @@
       <c r="H20" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>10</v>
       </c>
@@ -1301,8 +1436,11 @@
       <c r="H21" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>11</v>
       </c>
@@ -1325,10 +1463,13 @@
         <v>117</v>
       </c>
       <c r="H22" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="I22" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>11</v>
       </c>
@@ -1351,7 +1492,10 @@
         <v>112</v>
       </c>
       <c r="H23" t="s">
-        <v>119</v>
+        <v>118</v>
+      </c>
+      <c r="I23" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add hashcodes for each speaker
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\ithacapublicworks.github.io\generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\public works\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FB780F-BA03-4DBE-9938-A37CDB59B5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFBC8D5-BB49-41CB-AD72-530F6DAE6462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="0" windowWidth="19180" windowHeight="10080" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="167">
   <si>
     <t>speaker</t>
   </si>
@@ -456,6 +456,87 @@
   </si>
   <si>
     <t>a ghostwriting</t>
+  </si>
+  <si>
+    <t>hashcode</t>
+  </si>
+  <si>
+    <t>zachulibarri</t>
+  </si>
+  <si>
+    <t>evesnyder</t>
+  </si>
+  <si>
+    <t>jamesnagy</t>
+  </si>
+  <si>
+    <t>benfried</t>
+  </si>
+  <si>
+    <t>ligiacoelho</t>
+  </si>
+  <si>
+    <t>meganbarrington</t>
+  </si>
+  <si>
+    <t>sethstrickland</t>
+  </si>
+  <si>
+    <t>danielasamur</t>
+  </si>
+  <si>
+    <t>lukekeller</t>
+  </si>
+  <si>
+    <t>hunteradams</t>
+  </si>
+  <si>
+    <t>michaelcaporizzo</t>
+  </si>
+  <si>
+    <t>mollyryan</t>
+  </si>
+  <si>
+    <t>karlsmolenski</t>
+  </si>
+  <si>
+    <t>daisyrosas</t>
+  </si>
+  <si>
+    <t>alisonritterhaus</t>
+  </si>
+  <si>
+    <t>zachulibarri2</t>
+  </si>
+  <si>
+    <t>adamhawkins</t>
+  </si>
+  <si>
+    <t>jayleeming</t>
+  </si>
+  <si>
+    <t>danielsprocket</t>
+  </si>
+  <si>
+    <t>heatherhuson</t>
+  </si>
+  <si>
+    <t>alitahoward</t>
+  </si>
+  <si>
+    <t>jimmyjordan</t>
+  </si>
+  <si>
+    <t>adamhowell</t>
+  </si>
+  <si>
+    <t>madisonfitzpatrick</t>
+  </si>
+  <si>
+    <t>andresmontealegre</t>
+  </si>
+  <si>
+    <t>sethkoproski</t>
   </si>
 </sst>
 </file>
@@ -491,9 +572,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,7 +594,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -808,15 +890,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F859F76-284E-4154-B5CC-2AAD28AB7940}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -841,8 +926,11 @@
       <c r="H1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I1" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -867,8 +955,11 @@
       <c r="H2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I2" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -893,8 +984,11 @@
       <c r="H3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I3" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -919,8 +1013,11 @@
       <c r="H4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I4" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -945,8 +1042,11 @@
       <c r="H5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I5" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -971,8 +1071,11 @@
       <c r="H6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I6" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -997,8 +1100,11 @@
       <c r="H7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I7" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1023,8 +1129,11 @@
       <c r="H8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I8" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1049,8 +1158,11 @@
       <c r="H9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I9" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -1075,8 +1187,11 @@
       <c r="H10" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I10" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1101,8 +1216,11 @@
       <c r="H11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I11" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -1127,8 +1245,11 @@
       <c r="H12" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I12" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1153,8 +1274,11 @@
       <c r="H13" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I13" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1179,8 +1303,11 @@
       <c r="H14" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I14" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
@@ -1205,8 +1332,11 @@
       <c r="H15" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I15" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1231,8 +1361,11 @@
       <c r="H16" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I16" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>8</v>
       </c>
@@ -1257,8 +1390,11 @@
       <c r="H17" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I17" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>9</v>
       </c>
@@ -1283,8 +1419,11 @@
       <c r="H18" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I18" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>9</v>
       </c>
@@ -1309,8 +1448,11 @@
       <c r="H19" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I19" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>10</v>
       </c>
@@ -1335,8 +1477,11 @@
       <c r="H20" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I20" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>10</v>
       </c>
@@ -1361,8 +1506,11 @@
       <c r="H21" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I21" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>11</v>
       </c>
@@ -1387,8 +1535,11 @@
       <c r="H22" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I22" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>11</v>
       </c>
@@ -1413,8 +1564,11 @@
       <c r="H23" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I23" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>12</v>
       </c>
@@ -1439,8 +1593,11 @@
       <c r="H24" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I24" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>12</v>
       </c>
@@ -1465,8 +1622,11 @@
       <c r="H25" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>13</v>
       </c>
@@ -1491,8 +1651,11 @@
       <c r="H26" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I26" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>13</v>
       </c>
@@ -1516,6 +1679,9 @@
       </c>
       <c r="H27" t="s">
         <v>137</v>
+      </c>
+      <c r="I27" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added bios and titles for November talk
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\public works\ithacapublicworks.github.io\generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFBC8D5-BB49-41CB-AD72-530F6DAE6462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE04DE62-7756-4052-94E3-3A0C6E38BF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
+    <workbookView xWindow="10" yWindow="0" windowWidth="19180" windowHeight="10080" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="169">
   <si>
     <t>speaker</t>
   </si>
@@ -449,12 +449,6 @@
     <t>a psychology</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Title coming soon!</t>
-  </si>
-  <si>
     <t>a ghostwriting</t>
   </si>
   <si>
@@ -537,6 +531,18 @@
   </si>
   <si>
     <t>sethkoproski</t>
+  </si>
+  <si>
+    <t>Ghostwriting: An Insider's View of an Invisible Profession</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ever wonder how others perceive you based on your actions? We all do. Shockingly, recent studies in psychology reveal we're often quite mistaken about these perceptions. For example, people think they're less liked by others than they actually are, or they assume others aren't interested in their unsolicited advice when in fact they are. Such findings could help us get along better with others. But how accurate are these studies? And is it possible that participants in these studies are just trying to appear 'nice' when answering research questions? In this talk, I'll share my own research on this topic and discuss if we should take these findings at face value. Join me to discuss the fascinating, messy world of how we're seen by others.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ghostwriting often gets a bad rap as a cop-out for politicians and celebrities who are too lazy to write their own books. But the truth is, ghostwriting is more common than ever, and for many authors, it's no longer the shameful secret it once was. So, who actually hires ghostwriters? What do ghostwriters really do? And what's the future of this ancient profession in a world of generative AI? </t>
+  </si>
+  <si>
+    <t>Can You Accurately Perceive How Others Think About You?</t>
   </si>
 </sst>
 </file>
@@ -572,10 +578,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,7 +599,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -892,16 +897,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F859F76-284E-4154-B5CC-2AAD28AB7940}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24.81640625" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -926,11 +932,11 @@
       <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -955,11 +961,11 @@
       <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -984,11 +990,11 @@
       <c r="H3" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1013,11 +1019,11 @@
       <c r="H4" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1042,11 +1048,11 @@
       <c r="H5" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1071,11 +1077,11 @@
       <c r="H6" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1100,11 +1106,11 @@
       <c r="H7" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1129,11 +1135,11 @@
       <c r="H8" t="s">
         <v>42</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1158,11 +1164,11 @@
       <c r="H9" t="s">
         <v>43</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>5</v>
       </c>
@@ -1187,11 +1193,11 @@
       <c r="H10" t="s">
         <v>51</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1216,11 +1222,11 @@
       <c r="H11" t="s">
         <v>52</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>6</v>
       </c>
@@ -1245,11 +1251,11 @@
       <c r="H12" t="s">
         <v>64</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1274,11 +1280,11 @@
       <c r="H13" t="s">
         <v>76</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1303,11 +1309,11 @@
       <c r="H14" t="s">
         <v>72</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>7</v>
       </c>
@@ -1332,11 +1338,11 @@
       <c r="H15" t="s">
         <v>73</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1361,11 +1367,11 @@
       <c r="H16" t="s">
         <v>89</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>8</v>
       </c>
@@ -1390,11 +1396,11 @@
       <c r="H17" t="s">
         <v>90</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>9</v>
       </c>
@@ -1419,11 +1425,11 @@
       <c r="H18" t="s">
         <v>114</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>9</v>
       </c>
@@ -1448,11 +1454,11 @@
       <c r="H19" t="s">
         <v>113</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>10</v>
       </c>
@@ -1477,11 +1483,11 @@
       <c r="H20" t="s">
         <v>104</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>10</v>
       </c>
@@ -1506,11 +1512,11 @@
       <c r="H21" t="s">
         <v>105</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>11</v>
       </c>
@@ -1535,11 +1541,11 @@
       <c r="H22" t="s">
         <v>118</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>11</v>
       </c>
@@ -1564,11 +1570,11 @@
       <c r="H23" t="s">
         <v>119</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>12</v>
       </c>
@@ -1594,10 +1600,10 @@
         <v>130</v>
       </c>
       <c r="I24" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>12</v>
       </c>
@@ -1623,10 +1629,10 @@
         <v>122</v>
       </c>
       <c r="I25" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>13</v>
       </c>
@@ -1643,19 +1649,19 @@
         <v>135</v>
       </c>
       <c r="F26" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G26" t="s">
-        <v>138</v>
+        <v>165</v>
       </c>
       <c r="H26" t="s">
-        <v>137</v>
+        <v>167</v>
       </c>
       <c r="I26" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>13</v>
       </c>
@@ -1675,13 +1681,13 @@
         <v>136</v>
       </c>
       <c r="G27" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
       <c r="H27" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="I27" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed spelling error for Andrés' name
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE04DE62-7756-4052-94E3-3A0C6E38BF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6823ABC2-4853-40DA-8FD9-95E5D0696E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10" yWindow="0" windowWidth="19180" windowHeight="10080" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
@@ -437,9 +437,6 @@
     <t>Madison Fitzpatrick</t>
   </si>
   <si>
-    <t>Andres Montealegre</t>
-  </si>
-  <si>
     <t>PhD Candidate in the Cornell Psychology Dept.</t>
   </si>
   <si>
@@ -543,6 +540,9 @@
   </si>
   <si>
     <t>Can You Accurately Perceive How Others Think About You?</t>
+  </si>
+  <si>
+    <t>Andrés Montealegre</t>
   </si>
 </sst>
 </file>
@@ -898,7 +898,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -933,7 +933,7 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -962,7 +962,7 @@
         <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -991,7 +991,7 @@
         <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -1020,7 +1020,7 @@
         <v>23</v>
       </c>
       <c r="I4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1049,7 +1049,7 @@
         <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -1078,7 +1078,7 @@
         <v>33</v>
       </c>
       <c r="I6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -1107,7 +1107,7 @@
         <v>34</v>
       </c>
       <c r="I7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -1136,7 +1136,7 @@
         <v>42</v>
       </c>
       <c r="I8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -1165,7 +1165,7 @@
         <v>43</v>
       </c>
       <c r="I9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -1194,7 +1194,7 @@
         <v>51</v>
       </c>
       <c r="I10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -1223,7 +1223,7 @@
         <v>52</v>
       </c>
       <c r="I11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -1252,7 +1252,7 @@
         <v>64</v>
       </c>
       <c r="I12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -1281,7 +1281,7 @@
         <v>76</v>
       </c>
       <c r="I13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -1310,7 +1310,7 @@
         <v>72</v>
       </c>
       <c r="I14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -1339,7 +1339,7 @@
         <v>73</v>
       </c>
       <c r="I15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -1368,7 +1368,7 @@
         <v>89</v>
       </c>
       <c r="I16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -1397,7 +1397,7 @@
         <v>90</v>
       </c>
       <c r="I17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -1426,7 +1426,7 @@
         <v>114</v>
       </c>
       <c r="I18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -1455,7 +1455,7 @@
         <v>113</v>
       </c>
       <c r="I19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -1484,7 +1484,7 @@
         <v>104</v>
       </c>
       <c r="I20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -1513,7 +1513,7 @@
         <v>105</v>
       </c>
       <c r="I21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -1542,7 +1542,7 @@
         <v>118</v>
       </c>
       <c r="I22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -1571,7 +1571,7 @@
         <v>119</v>
       </c>
       <c r="I23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
@@ -1600,7 +1600,7 @@
         <v>130</v>
       </c>
       <c r="I24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -1629,7 +1629,7 @@
         <v>122</v>
       </c>
       <c r="I25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -1646,19 +1646,19 @@
         <v>132</v>
       </c>
       <c r="E26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G26" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
@@ -1672,22 +1672,22 @@
         <v>2023</v>
       </c>
       <c r="D27" t="s">
+        <v>168</v>
+      </c>
+      <c r="E27" t="s">
         <v>133</v>
       </c>
-      <c r="E27" t="s">
-        <v>134</v>
-      </c>
       <c r="F27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G27" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Toni Alimi's abstract and title
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77933DF3-3415-4CC2-A961-28DF01C4DB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD65FD0-7361-4A74-884C-6003CB4C6571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10" yWindow="0" windowWidth="19180" windowHeight="10080" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
@@ -551,21 +551,12 @@
     <t>Not All is Lost: How Public Gardens are (Attempting to) Save the World</t>
   </si>
   <si>
-    <t>Do you find yourself freaking out over the state of the global environment, climate change, and loss of biodiversity? If so, you’re not alone- eco-anxiety has become one of the leading mental health issues in the third decade of the 21st century. Public gardens, which include botanic gardens, arboreta, conservatories, and historic landscapes, are addressing these seemingly overwhelming environmental challenges through their extensive collections, protection of natural areas, preservation of endangered species, and through programming and messaging. Will public gardens single-handedly solve all of these problems? No, but they can be a significant contributor to the solutions. In this talk you’ll learn some of the ways they are making a difference.</t>
-  </si>
-  <si>
     <t>Dr. Donald A. Rakow</t>
   </si>
   <si>
     <t>a Classics and philosophy</t>
   </si>
   <si>
-    <t>Title Coming Soon!</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Dr. Toni Alimi</t>
   </si>
   <si>
@@ -582,6 +573,15 @@
   </si>
   <si>
     <t>Associate Professor (retired) in the  School of Integrative Plant Science at Cornell University</t>
+  </si>
+  <si>
+    <t>Justifying Slavery: The Intellectual Background of the Reconstruction Amendments</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Recent appraisals of the Thirteenth Amendment to the United States Constitution often note with alarm that slavery remains a legal form of punishment and lament for how this loophole has been weaponized against black Americans. I’m interested in how this alarm reflects an Aristotelian attitude towards slavery (more on what that means in the talk!), and about how an intellectual history of various justifications for slavery can help us understand what’s going on in the Thirteenth Amendment.</t>
+  </si>
+  <si>
+    <t>Do you find yourself freaking out over the state of the global environment, climate change, and loss of biodiversity? If so, you’re not alone — eco-anxiety has become one of the leading mental health issues in the third decade of the 21st century. Public gardens, which include botanic gardens, arboreta, conservatories, and historic landscapes, are addressing these seemingly overwhelming environmental challenges through their extensive collections, protection of natural areas, preservation of endangered species, and through programming and messaging. Will public gardens single-handedly solve all of these problems? No, but they can be a significant contributor to the solutions. In this talk you’ll learn some of the ways they are making a difference.</t>
   </si>
 </sst>
 </file>
@@ -939,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F859F76-284E-4154-B5CC-2AAD28AB7940}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1743,22 +1743,22 @@
         <v>2023</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E28" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F28" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G28" t="s">
         <v>170</v>
       </c>
       <c r="H28" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="I28" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
@@ -1772,22 +1772,22 @@
         <v>2023</v>
       </c>
       <c r="D29" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E29" t="s">
+        <v>177</v>
+      </c>
+      <c r="F29" t="s">
+        <v>172</v>
+      </c>
+      <c r="G29" t="s">
+        <v>179</v>
+      </c>
+      <c r="H29" t="s">
         <v>180</v>
       </c>
-      <c r="F29" t="s">
-        <v>173</v>
-      </c>
-      <c r="G29" t="s">
-        <v>174</v>
-      </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>175</v>
-      </c>
-      <c r="I29" t="s">
-        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test added Jimmy Jordan photo
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD65FD0-7361-4A74-884C-6003CB4C6571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5932A2F-FC35-44A5-B0C0-2128BDDC6142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10" yWindow="0" windowWidth="19180" windowHeight="10080" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
@@ -428,9 +428,6 @@
     <t>Where the Media Death Spiral Brought Us: The Decline of Local Reporting, and an Industry Looking for its Footing</t>
   </si>
   <si>
-    <t xml:space="preserve">The newspaper industry in the U.S. has been undergoing a significant decline since the early 2000s. The rise of the internet ushered in an era of information abundance and accessibility. However, this transition has severely impacted the traditional business models that once supported local newspapers, resulting in noticeable gaps in community coverage across the country. All of this is set against a climate where trust in media is approaching historic lows in the U.S.&lt;br&gt;&lt;br&gt;This presentation will illustrate these challenges, both on a local scale and within a broader context. Additionally, we will delve into the new models that are being explored in an effort to revitalize local reporting. </t>
-  </si>
-  <si>
     <t>November 1st</t>
   </si>
   <si>
@@ -582,6 +579,9 @@
   </si>
   <si>
     <t>Do you find yourself freaking out over the state of the global environment, climate change, and loss of biodiversity? If so, you’re not alone — eco-anxiety has become one of the leading mental health issues in the third decade of the 21st century. Public gardens, which include botanic gardens, arboreta, conservatories, and historic landscapes, are addressing these seemingly overwhelming environmental challenges through their extensive collections, protection of natural areas, preservation of endangered species, and through programming and messaging. Will public gardens single-handedly solve all of these problems? No, but they can be a significant contributor to the solutions. In this talk you’ll learn some of the ways they are making a difference.</t>
+  </si>
+  <si>
+    <t>The newspaper industry in the U.S. has been undergoing a significant decline since the early 2000s. The rise of the internet ushered in an era of information abundance and accessibility. However, this transition has severely impacted the traditional business models that once supported local newspapers, resulting in noticeable gaps in community coverage across the country. All of this is set against a climate where trust in media is approaching historic lows in the U.S.&lt;br&gt;&lt;br&gt;This presentation will illustrate these challenges, both on a local scale and within a broader context. Additionally, we will delve into the new models that are being explored in an effort to revitalize local reporting. &lt;br&gt;&lt;br&gt;&lt;div class="box"&gt; &lt;img src="Oct_4_2023_Jimmy_Jordan_1.jpg" style = 'width: 550' class='center'&gt; &lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -939,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F859F76-284E-4154-B5CC-2AAD28AB7940}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -975,7 +975,7 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -1004,7 +1004,7 @@
         <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1033,7 +1033,7 @@
         <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -1062,7 +1062,7 @@
         <v>23</v>
       </c>
       <c r="I4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1091,7 +1091,7 @@
         <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -1120,7 +1120,7 @@
         <v>33</v>
       </c>
       <c r="I6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -1149,7 +1149,7 @@
         <v>34</v>
       </c>
       <c r="I7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -1178,7 +1178,7 @@
         <v>42</v>
       </c>
       <c r="I8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -1207,7 +1207,7 @@
         <v>43</v>
       </c>
       <c r="I9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -1236,7 +1236,7 @@
         <v>51</v>
       </c>
       <c r="I10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -1265,7 +1265,7 @@
         <v>52</v>
       </c>
       <c r="I11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -1294,7 +1294,7 @@
         <v>64</v>
       </c>
       <c r="I12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -1323,7 +1323,7 @@
         <v>76</v>
       </c>
       <c r="I13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -1352,7 +1352,7 @@
         <v>72</v>
       </c>
       <c r="I14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -1381,7 +1381,7 @@
         <v>73</v>
       </c>
       <c r="I15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -1410,7 +1410,7 @@
         <v>89</v>
       </c>
       <c r="I16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -1439,7 +1439,7 @@
         <v>90</v>
       </c>
       <c r="I17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -1468,7 +1468,7 @@
         <v>114</v>
       </c>
       <c r="I18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -1497,7 +1497,7 @@
         <v>113</v>
       </c>
       <c r="I19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -1526,7 +1526,7 @@
         <v>104</v>
       </c>
       <c r="I20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -1555,7 +1555,7 @@
         <v>105</v>
       </c>
       <c r="I21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -1584,7 +1584,7 @@
         <v>118</v>
       </c>
       <c r="I22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -1613,7 +1613,7 @@
         <v>119</v>
       </c>
       <c r="I23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
@@ -1639,10 +1639,10 @@
         <v>129</v>
       </c>
       <c r="H24" t="s">
-        <v>130</v>
+        <v>181</v>
       </c>
       <c r="I24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -1671,7 +1671,7 @@
         <v>122</v>
       </c>
       <c r="I25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -1679,28 +1679,28 @@
         <v>13</v>
       </c>
       <c r="B26" t="s">
+        <v>130</v>
+      </c>
+      <c r="C26">
+        <v>2023</v>
+      </c>
+      <c r="D26" t="s">
         <v>131</v>
       </c>
-      <c r="C26">
-        <v>2023</v>
-      </c>
-      <c r="D26" t="s">
-        <v>132</v>
-      </c>
       <c r="E26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G26" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I26" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
@@ -1708,28 +1708,28 @@
         <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C27">
         <v>2023</v>
       </c>
       <c r="D27" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
@@ -1737,28 +1737,28 @@
         <v>14</v>
       </c>
       <c r="B28" t="s">
+        <v>168</v>
+      </c>
+      <c r="C28">
+        <v>2023</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E28" t="s">
+        <v>177</v>
+      </c>
+      <c r="F28" t="s">
+        <v>175</v>
+      </c>
+      <c r="G28" t="s">
         <v>169</v>
       </c>
-      <c r="C28">
-        <v>2023</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E28" t="s">
-        <v>178</v>
-      </c>
-      <c r="F28" t="s">
-        <v>176</v>
-      </c>
-      <c r="G28" t="s">
-        <v>170</v>
-      </c>
       <c r="H28" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I28" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
@@ -1766,28 +1766,28 @@
         <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C29">
         <v>2023</v>
       </c>
       <c r="D29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G29" t="s">
+        <v>178</v>
+      </c>
+      <c r="H29" t="s">
         <v>179</v>
       </c>
-      <c r="H29" t="s">
-        <v>180</v>
-      </c>
       <c r="I29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test added Jimmy Jordan photo file
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5932A2F-FC35-44A5-B0C0-2128BDDC6142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF9B4A0-8C49-44FB-9273-E8DAF2A43772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10" yWindow="0" windowWidth="19180" windowHeight="10080" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
@@ -581,7 +581,7 @@
     <t>Do you find yourself freaking out over the state of the global environment, climate change, and loss of biodiversity? If so, you’re not alone — eco-anxiety has become one of the leading mental health issues in the third decade of the 21st century. Public gardens, which include botanic gardens, arboreta, conservatories, and historic landscapes, are addressing these seemingly overwhelming environmental challenges through their extensive collections, protection of natural areas, preservation of endangered species, and through programming and messaging. Will public gardens single-handedly solve all of these problems? No, but they can be a significant contributor to the solutions. In this talk you’ll learn some of the ways they are making a difference.</t>
   </si>
   <si>
-    <t>The newspaper industry in the U.S. has been undergoing a significant decline since the early 2000s. The rise of the internet ushered in an era of information abundance and accessibility. However, this transition has severely impacted the traditional business models that once supported local newspapers, resulting in noticeable gaps in community coverage across the country. All of this is set against a climate where trust in media is approaching historic lows in the U.S.&lt;br&gt;&lt;br&gt;This presentation will illustrate these challenges, both on a local scale and within a broader context. Additionally, we will delve into the new models that are being explored in an effort to revitalize local reporting. &lt;br&gt;&lt;br&gt;&lt;div class="box"&gt; &lt;img src="Oct_4_2023_Jimmy_Jordan_1.jpg" style = 'width: 550' class='center'&gt; &lt;/div&gt;</t>
+    <t>The newspaper industry in the U.S. has been undergoing a significant decline since the early 2000s. The rise of the internet ushered in an era of information abundance and accessibility. However, this transition has severely impacted the traditional business models that once supported local newspapers, resulting in noticeable gaps in community coverage across the country. All of this is set against a climate where trust in media is approaching historic lows in the U.S.&lt;br&gt;&lt;br&gt;This presentation will illustrate these challenges, both on a local scale and within a broader context. Additionally, we will delve into the new models that are being explored in an effort to revitalize local reporting. &lt;br&gt;&lt;br&gt;&lt;div class="box"&gt; &lt;img src="images/Oct_4_2023_Jimmy_Jordan_1.jpg" style = 'width: 550' class='center'&gt; &lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -940,7 +940,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
test added Jordan photo
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF9B4A0-8C49-44FB-9273-E8DAF2A43772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65C95C8-5A0B-45F6-8A19-C0A3F34EE79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10" yWindow="0" windowWidth="19180" windowHeight="10080" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
@@ -581,7 +581,7 @@
     <t>Do you find yourself freaking out over the state of the global environment, climate change, and loss of biodiversity? If so, you’re not alone — eco-anxiety has become one of the leading mental health issues in the third decade of the 21st century. Public gardens, which include botanic gardens, arboreta, conservatories, and historic landscapes, are addressing these seemingly overwhelming environmental challenges through their extensive collections, protection of natural areas, preservation of endangered species, and through programming and messaging. Will public gardens single-handedly solve all of these problems? No, but they can be a significant contributor to the solutions. In this talk you’ll learn some of the ways they are making a difference.</t>
   </si>
   <si>
-    <t>The newspaper industry in the U.S. has been undergoing a significant decline since the early 2000s. The rise of the internet ushered in an era of information abundance and accessibility. However, this transition has severely impacted the traditional business models that once supported local newspapers, resulting in noticeable gaps in community coverage across the country. All of this is set against a climate where trust in media is approaching historic lows in the U.S.&lt;br&gt;&lt;br&gt;This presentation will illustrate these challenges, both on a local scale and within a broader context. Additionally, we will delve into the new models that are being explored in an effort to revitalize local reporting. &lt;br&gt;&lt;br&gt;&lt;div class="box"&gt; &lt;img src="images/Oct_4_2023_Jimmy_Jordan_1.jpg" style = 'width: 550' class='center'&gt; &lt;/div&gt;</t>
+    <t>The newspaper industry in the U.S. has been undergoing a significant decline since the early 2000s. The rise of the internet ushered in an era of information abundance and accessibility. However, this transition has severely impacted the traditional business models that once supported local newspapers, resulting in noticeable gaps in community coverage across the country. All of this is set against a climate where trust in media is approaching historic lows in the U.S.&lt;br&gt;&lt;br&gt;This presentation will illustrate these challenges, both on a local scale and within a broader context. Additionally, we will delve into the new models that are being explored in an effort to revitalize local reporting.&lt;br&gt;&lt;br&gt;&lt;div class="box"&gt; &lt;img src="images/Oct_4_2023_Jimmy_Jordan_1.jpg" style = 'width: 550' class='center'&gt; &lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -940,7 +940,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
added rest of oct and nov photos
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65C95C8-5A0B-45F6-8A19-C0A3F34EE79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EEDCAA0-0F6F-4B55-AB19-7441237C7C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10" yWindow="0" windowWidth="19180" windowHeight="10080" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
@@ -404,9 +404,6 @@
     <t>Adam Howell</t>
   </si>
   <si>
-    <t>Everyone is aware of the price of food – from kitchen tables to restaurant counters, food costs impact our lives in profound ways. But another, less understood cost associated with our food is born out of the pressures faced by farmers as they struggle to succeed working in one of the most unforgiving industries in America. Farmers deal with numerous stressors outside of their control including market pressures, weather, price increases, supplies, and many more. Furthermore, farmers deal with the geographic challenge of being isolated from support services in rural areas, and cultural/psychological challenges stemming from personal stigmas against seeking help.&lt;br&gt;&lt;br&gt;In this Public Works talk, learn about a unique program in NYS that provides free, confidential support for farmers to help with any number of issues they may face. NY FarmNet approaches farm assistance and support through a “holistic” model by deploying a consultant team representing both the personal and financial aspects of every challenge.</t>
-  </si>
-  <si>
     <t>For Whom the Dinner Bell Tolls: The Struggles of America’s Farming Community and How NY FarmNet Helps</t>
   </si>
   <si>
@@ -530,12 +527,6 @@
     <t>Ghostwriting: An Insider's View of an Invisible Profession</t>
   </si>
   <si>
-    <t xml:space="preserve"> Ever wonder how others perceive you based on your actions? We all do. Shockingly, recent studies in psychology reveal we're often quite mistaken about these perceptions. For example, people think they're less liked by others than they actually are, or they assume others aren't interested in their unsolicited advice when in fact they are. Such findings could help us get along better with others. But how accurate are these studies? And is it possible that participants in these studies are just trying to appear 'nice' when answering research questions? In this talk, I'll share my own research on this topic and discuss if we should take these findings at face value. Join me to discuss the fascinating, messy world of how we're seen by others.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ghostwriting often gets a bad rap as a cop-out for politicians and celebrities who are too lazy to write their own books. But the truth is, ghostwriting is more common than ever, and for many authors, it's no longer the shameful secret it once was. So, who actually hires ghostwriters? What do ghostwriters really do? And what's the future of this ancient profession in a world of generative AI? </t>
-  </si>
-  <si>
     <t>Can You Accurately Perceive How Others Think About You?</t>
   </si>
   <si>
@@ -582,6 +573,15 @@
   </si>
   <si>
     <t>The newspaper industry in the U.S. has been undergoing a significant decline since the early 2000s. The rise of the internet ushered in an era of information abundance and accessibility. However, this transition has severely impacted the traditional business models that once supported local newspapers, resulting in noticeable gaps in community coverage across the country. All of this is set against a climate where trust in media is approaching historic lows in the U.S.&lt;br&gt;&lt;br&gt;This presentation will illustrate these challenges, both on a local scale and within a broader context. Additionally, we will delve into the new models that are being explored in an effort to revitalize local reporting.&lt;br&gt;&lt;br&gt;&lt;div class="box"&gt; &lt;img src="images/Oct_4_2023_Jimmy_Jordan_1.jpg" style = 'width: 550' class='center'&gt; &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Everyone is aware of the price of food – from kitchen tables to restaurant counters, food costs impact our lives in profound ways. But another, less understood cost associated with our food is born out of the pressures faced by farmers as they struggle to succeed working in one of the most unforgiving industries in America. Farmers deal with numerous stressors outside of their control including market pressures, weather, price increases, supplies, and many more. Furthermore, farmers deal with the geographic challenge of being isolated from support services in rural areas, and cultural/psychological challenges stemming from personal stigmas against seeking help.&lt;br&gt;&lt;br&gt;In this Public Works talk, learn about a unique program in NYS that provides free, confidential support for farmers to help with any number of issues they may face. NY FarmNet approaches farm assistance and support through a “holistic” model by deploying a consultant team representing both the personal and financial aspects of every challenge.&lt;br&gt;&lt;br&gt;&lt;div class="box"&gt; &lt;img src="images/Oct_4_2023_Adam_Howell_1.jpg" style = 'width: 550' class='center'&gt; &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ghostwriting often gets a bad rap as a cop-out for politicians and celebrities who are too lazy to write their own books. But the truth is, ghostwriting is more common than ever, and for many authors, it's no longer the shameful secret it once was. So, who actually hires ghostwriters? What do ghostwriters really do? And what's the future of this ancient profession in a world of generative AI?&lt;br&gt;&lt;br&gt;&lt;div class="box"&gt; &lt;img src="images/Nov_1_2023_Madison_Fitzpatrick_2.jpg" style = 'width: 550' class='center'&gt; &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ever wonder how others perceive you based on your actions? We all do. Shockingly, recent studies in psychology reveal we're often quite mistaken about these perceptions. For example, people think they're less liked by others than they actually are, or they assume others aren't interested in their unsolicited advice when in fact they are. Such findings could help us get along better with others. But how accurate are these studies? And is it possible that participants in these studies are just trying to appear 'nice' when answering research questions? In this talk, I'll share my own research on this topic and discuss if we should take these findings at face value. Join me to discuss the fascinating, messy world of how we're seen by others.&lt;br&gt;&lt;br&gt;&lt;div class="box"&gt; &lt;img src="images/Nov_1_2023_Andres_Montealegre_1.jpg" style = 'width: 550' class='center'&gt; &lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -940,7 +940,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -975,7 +975,7 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -1004,7 +1004,7 @@
         <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1033,7 +1033,7 @@
         <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -1062,7 +1062,7 @@
         <v>23</v>
       </c>
       <c r="I4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1091,7 +1091,7 @@
         <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -1120,7 +1120,7 @@
         <v>33</v>
       </c>
       <c r="I6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -1149,7 +1149,7 @@
         <v>34</v>
       </c>
       <c r="I7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -1178,7 +1178,7 @@
         <v>42</v>
       </c>
       <c r="I8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -1207,7 +1207,7 @@
         <v>43</v>
       </c>
       <c r="I9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -1236,7 +1236,7 @@
         <v>51</v>
       </c>
       <c r="I10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -1265,7 +1265,7 @@
         <v>52</v>
       </c>
       <c r="I11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -1294,7 +1294,7 @@
         <v>64</v>
       </c>
       <c r="I12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -1323,7 +1323,7 @@
         <v>76</v>
       </c>
       <c r="I13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -1352,7 +1352,7 @@
         <v>72</v>
       </c>
       <c r="I14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -1381,7 +1381,7 @@
         <v>73</v>
       </c>
       <c r="I15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -1410,7 +1410,7 @@
         <v>89</v>
       </c>
       <c r="I16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -1439,7 +1439,7 @@
         <v>90</v>
       </c>
       <c r="I17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -1468,7 +1468,7 @@
         <v>114</v>
       </c>
       <c r="I18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -1497,7 +1497,7 @@
         <v>113</v>
       </c>
       <c r="I19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -1526,7 +1526,7 @@
         <v>104</v>
       </c>
       <c r="I20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -1555,7 +1555,7 @@
         <v>105</v>
       </c>
       <c r="I21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -1584,7 +1584,7 @@
         <v>118</v>
       </c>
       <c r="I22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -1613,7 +1613,7 @@
         <v>119</v>
       </c>
       <c r="I23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
@@ -1627,22 +1627,22 @@
         <v>2023</v>
       </c>
       <c r="D24" t="s">
+        <v>125</v>
+      </c>
+      <c r="E24" t="s">
         <v>126</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>127</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>128</v>
       </c>
-      <c r="G24" t="s">
-        <v>129</v>
-      </c>
       <c r="H24" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I24" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -1659,19 +1659,19 @@
         <v>121</v>
       </c>
       <c r="E25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H25" t="s">
-        <v>122</v>
+        <v>179</v>
       </c>
       <c r="I25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -1679,28 +1679,28 @@
         <v>13</v>
       </c>
       <c r="B26" t="s">
+        <v>129</v>
+      </c>
+      <c r="C26">
+        <v>2023</v>
+      </c>
+      <c r="D26" t="s">
         <v>130</v>
       </c>
-      <c r="C26">
-        <v>2023</v>
-      </c>
-      <c r="D26" t="s">
-        <v>131</v>
-      </c>
       <c r="E26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H26" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="I26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
@@ -1708,28 +1708,28 @@
         <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C27">
         <v>2023</v>
       </c>
       <c r="D27" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G27" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H27" t="s">
-        <v>164</v>
+        <v>181</v>
       </c>
       <c r="I27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
@@ -1737,28 +1737,28 @@
         <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C28">
         <v>2023</v>
       </c>
       <c r="D28" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E28" t="s">
+        <v>174</v>
+      </c>
+      <c r="F28" t="s">
+        <v>172</v>
+      </c>
+      <c r="G28" t="s">
+        <v>166</v>
+      </c>
+      <c r="H28" t="s">
+        <v>177</v>
+      </c>
+      <c r="I28" t="s">
         <v>170</v>
-      </c>
-      <c r="E28" t="s">
-        <v>177</v>
-      </c>
-      <c r="F28" t="s">
-        <v>175</v>
-      </c>
-      <c r="G28" t="s">
-        <v>169</v>
-      </c>
-      <c r="H28" t="s">
-        <v>180</v>
-      </c>
-      <c r="I28" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
@@ -1766,28 +1766,28 @@
         <v>14</v>
       </c>
       <c r="B29" t="s">
+        <v>165</v>
+      </c>
+      <c r="C29">
+        <v>2023</v>
+      </c>
+      <c r="D29" t="s">
+        <v>169</v>
+      </c>
+      <c r="E29" t="s">
+        <v>173</v>
+      </c>
+      <c r="F29" t="s">
         <v>168</v>
       </c>
-      <c r="C29">
-        <v>2023</v>
-      </c>
-      <c r="D29" t="s">
-        <v>172</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="G29" t="s">
+        <v>175</v>
+      </c>
+      <c r="H29" t="s">
         <v>176</v>
       </c>
-      <c r="F29" t="s">
+      <c r="I29" t="s">
         <v>171</v>
-      </c>
-      <c r="G29" t="s">
-        <v>178</v>
-      </c>
-      <c r="H29" t="s">
-        <v>179</v>
-      </c>
-      <c r="I29" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing Jimmy Jordan's picture
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B291A1B2-8FF8-41E4-AC65-B2086A9DA14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE1E8EE-4C11-4C2E-BE36-CBBEE490528F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10" yWindow="0" windowWidth="19180" windowHeight="10080" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
@@ -393,9 +393,6 @@
     <t>The Story of Balto, an Elite Sled Dog: Through his Genome</t>
   </si>
   <si>
-    <t>Almost 100 years ago, Balto, along with a pack of elite sled dogs helped save the community of Nome, Alaska, from a diphtheria outbreak. Balto is representative of the sled dogs of the era who were reputed for their hardiness, endurance, and tolerance of harsh conditions at a time when northern communities relied on them for transportation, protection, and companionship. Unlike modern breeds, Balto and his contemporaries were products of generations of mating of diverse, outbred dogs selected for their performance and hardiness.  Today, Balto is immortalized with a statue in Central Park and is physically preserved and on display at the Cleaveland Museum of Natural History. We asked ourselves, could we use advances in genomic technologies and ancient DNA recovery techniques to parse through Balto’s DNA and understand selection emphasis and diversity occurring in sled dogs in the 1930’s? Could we decipher Balto’s physical appearance from his DNA and identify healthy developmental gene variants that may have endowed sled dogs in that era with abilities to withstand and thrive in harsh environments? Could we use our findings to guide modern breeders to breed healthier dogs? &lt;br&gt;&lt;br&gt;Also, here's a photo of Dr. Huson racing as a musher in Alaska!&lt;div class="box"&gt; &lt;img src="images/huson_sled.jpg" style = 'width: 550' class='center'&gt; &lt;/div&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">Have you seen curling on TV, that weird game with stones, and brooms, and people yelling at each other on ice?  Maybe you caught the fever back in 2018, watching the Men’s curling team win USA’s first gold medal in the sport, saw it in a movie, or have visited Canada at any point in your life.  Alita started curling with the Finger Lakes Curling Club in 2018 after taking one of the first Learn to Curl’s, soon after the club’s founding.  She currently skips, is an instructor, volunteers on the club’s board, and travels to friendlies and bonspiels to compete and meet other curlers.  In a Public Works’ version of broomstacking, Alita will talk about the history, explain the types and rules of curling, and delve a little into the science, all while taking part in a major part of curling: drinking beverages. </t>
   </si>
   <si>
@@ -573,9 +570,6 @@
     <t>Do you find yourself freaking out over the state of the global environment, climate change, and loss of biodiversity? If so, you’re not alone — eco-anxiety has become one of the leading mental health issues in the third decade of the 21st century. Public gardens, which include botanic gardens, arboreta, conservatories, and historic landscapes, are addressing these seemingly overwhelming environmental challenges through their extensive collections, protection of natural areas, preservation of endangered species, and through programming and messaging. Will public gardens single-handedly solve all of these problems? No, but they can be a significant contributor to the solutions. In this talk you’ll learn some of the ways they are making a difference.</t>
   </si>
   <si>
-    <t>The newspaper industry in the U.S. has been undergoing a significant decline since the early 2000s. The rise of the internet ushered in an era of information abundance and accessibility. However, this transition has severely impacted the traditional business models that once supported local newspapers, resulting in noticeable gaps in community coverage across the country. All of this is set against a climate where trust in media is approaching historic lows in the U.S.&lt;br&gt;&lt;br&gt;This presentation will illustrate these challenges, both on a local scale and within a broader context. Additionally, we will delve into the new models that are being explored in an effort to revitalize local reporting.&lt;br&gt;&lt;br&gt;&lt;div class="box"&gt; &lt;img src="images/Oct_4_2023_Jimmy_Jordan_1.jpg" style = 'width: 550' class='center'&gt; &lt;/div&gt;</t>
-  </si>
-  <si>
     <t>February 7th</t>
   </si>
   <si>
@@ -616,6 +610,12 @@
   </si>
   <si>
     <t>Everyone is aware of the price of food – from kitchen tables to restaurant counters, food costs impact our lives in profound ways. But another, less understood cost associated with our food is born out of the pressures faced by farmers as they struggle to succeed working in one of the most unforgiving industries in America. Farmers deal with numerous stressors outside of their control including market pressures, weather, price increases, supplies, and many more. Furthermore, farmers deal with the geographic challenge of being isolated from support services in rural areas, and cultural/psychological challenges stemming from personal stigmas against seeking help.&lt;br&gt;&lt;br&gt;In this Public Works talk, learn about a unique program in NYS that provides free, confidential support for farmers to help with any number of issues they may face. NY FarmNet approaches farm assistance and support through a “holistic” model by deploying a consultant team representing both the personal and financial aspects of every challenge.&lt;br&gt;&lt;br&gt;&lt;div class="box"&gt; &lt;img src="images/Oct_4_2023_Adam_Howell_1.jpg" class='center'&gt; &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Almost 100 years ago, Balto, along with a pack of elite sled dogs helped save the community of Nome, Alaska, from a diphtheria outbreak. Balto is representative of the sled dogs of the era who were reputed for their hardiness, endurance, and tolerance of harsh conditions at a time when northern communities relied on them for transportation, protection, and companionship. Unlike modern breeds, Balto and his contemporaries were products of generations of mating of diverse, outbred dogs selected for their performance and hardiness.  Today, Balto is immortalized with a statue in Central Park and is physically preserved and on display at the Cleaveland Museum of Natural History. We asked ourselves, could we use advances in genomic technologies and ancient DNA recovery techniques to parse through Balto’s DNA and understand selection emphasis and diversity occurring in sled dogs in the 1930’s? Could we decipher Balto’s physical appearance from his DNA and identify healthy developmental gene variants that may have endowed sled dogs in that era with abilities to withstand and thrive in harsh environments? Could we use our findings to guide modern breeders to breed healthier dogs? &lt;br&gt;&lt;br&gt;Also, here's a photo of Dr. Huson racing as a musher in Alaska!&lt;div class="box"&gt; &lt;img src="images/huson_sled.jpg" class='center'&gt; &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>The newspaper industry in the U.S. has been undergoing a significant decline since the early 2000s. The rise of the internet ushered in an era of information abundance and accessibility. However, this transition has severely impacted the traditional business models that once supported local newspapers, resulting in noticeable gaps in community coverage across the country. All of this is set against a climate where trust in media is approaching historic lows in the U.S.&lt;br&gt;&lt;br&gt;This presentation will illustrate these challenges, both on a local scale and within a broader context. Additionally, we will delve into the new models that are being explored in an effort to revitalize local reporting.&lt;br&gt;&lt;br&gt;&lt;div class="box"&gt; &lt;img src="images/Oct_4_2023_Jimmy_Jordan_1.jpg" style = 'width: 250' class='center'&gt; &lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -974,7 +974,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1009,7 +1009,7 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -1038,7 +1038,7 @@
         <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1067,7 +1067,7 @@
         <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -1096,7 +1096,7 @@
         <v>23</v>
       </c>
       <c r="I4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1125,7 +1125,7 @@
         <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -1154,7 +1154,7 @@
         <v>33</v>
       </c>
       <c r="I6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -1183,7 +1183,7 @@
         <v>34</v>
       </c>
       <c r="I7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -1212,7 +1212,7 @@
         <v>42</v>
       </c>
       <c r="I8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -1241,7 +1241,7 @@
         <v>43</v>
       </c>
       <c r="I9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -1270,7 +1270,7 @@
         <v>51</v>
       </c>
       <c r="I10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -1299,7 +1299,7 @@
         <v>52</v>
       </c>
       <c r="I11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -1328,7 +1328,7 @@
         <v>64</v>
       </c>
       <c r="I12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -1357,7 +1357,7 @@
         <v>76</v>
       </c>
       <c r="I13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -1386,7 +1386,7 @@
         <v>72</v>
       </c>
       <c r="I14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -1415,7 +1415,7 @@
         <v>73</v>
       </c>
       <c r="I15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -1444,7 +1444,7 @@
         <v>89</v>
       </c>
       <c r="I16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -1473,7 +1473,7 @@
         <v>90</v>
       </c>
       <c r="I17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -1502,7 +1502,7 @@
         <v>114</v>
       </c>
       <c r="I18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -1531,7 +1531,7 @@
         <v>113</v>
       </c>
       <c r="I19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -1560,7 +1560,7 @@
         <v>104</v>
       </c>
       <c r="I20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -1589,7 +1589,7 @@
         <v>105</v>
       </c>
       <c r="I21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -1615,10 +1615,10 @@
         <v>117</v>
       </c>
       <c r="H22" t="s">
-        <v>118</v>
+        <v>191</v>
       </c>
       <c r="I22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -1644,10 +1644,10 @@
         <v>112</v>
       </c>
       <c r="H23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
@@ -1655,28 +1655,28 @@
         <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C24">
         <v>2023</v>
       </c>
       <c r="D24" t="s">
+        <v>124</v>
+      </c>
+      <c r="E24" t="s">
         <v>125</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>126</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>127</v>
       </c>
-      <c r="G24" t="s">
-        <v>128</v>
-      </c>
       <c r="H24" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="I24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -1684,28 +1684,28 @@
         <v>12</v>
       </c>
       <c r="B25" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25">
+        <v>2023</v>
+      </c>
+      <c r="D25" t="s">
         <v>120</v>
       </c>
-      <c r="C25">
-        <v>2023</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
+        <v>123</v>
+      </c>
+      <c r="F25" t="s">
+        <v>122</v>
+      </c>
+      <c r="G25" t="s">
         <v>121</v>
       </c>
-      <c r="E25" t="s">
-        <v>124</v>
-      </c>
-      <c r="F25" t="s">
-        <v>123</v>
-      </c>
-      <c r="G25" t="s">
-        <v>122</v>
-      </c>
       <c r="H25" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -1713,28 +1713,28 @@
         <v>13</v>
       </c>
       <c r="B26" t="s">
+        <v>128</v>
+      </c>
+      <c r="C26">
+        <v>2023</v>
+      </c>
+      <c r="D26" t="s">
         <v>129</v>
       </c>
-      <c r="C26">
-        <v>2023</v>
-      </c>
-      <c r="D26" t="s">
-        <v>130</v>
-      </c>
       <c r="E26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H26" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
@@ -1742,28 +1742,28 @@
         <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C27">
         <v>2023</v>
       </c>
       <c r="D27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H27" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
@@ -1771,28 +1771,28 @@
         <v>14</v>
       </c>
       <c r="B28" t="s">
+        <v>164</v>
+      </c>
+      <c r="C28">
+        <v>2023</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E28" t="s">
+        <v>173</v>
+      </c>
+      <c r="F28" t="s">
+        <v>171</v>
+      </c>
+      <c r="G28" t="s">
         <v>165</v>
       </c>
-      <c r="C28">
-        <v>2023</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E28" t="s">
-        <v>174</v>
-      </c>
-      <c r="F28" t="s">
-        <v>172</v>
-      </c>
-      <c r="G28" t="s">
-        <v>166</v>
-      </c>
       <c r="H28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
@@ -1800,28 +1800,28 @@
         <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C29">
         <v>2023</v>
       </c>
       <c r="D29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G29" t="s">
+        <v>174</v>
+      </c>
+      <c r="H29" t="s">
         <v>175</v>
       </c>
-      <c r="H29" t="s">
-        <v>176</v>
-      </c>
       <c r="I29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
@@ -1829,28 +1829,28 @@
         <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C30">
         <v>2024</v>
       </c>
       <c r="D30" t="s">
+        <v>178</v>
+      </c>
+      <c r="E30" t="s">
+        <v>179</v>
+      </c>
+      <c r="F30" t="s">
         <v>180</v>
       </c>
-      <c r="E30" t="s">
+      <c r="G30" t="s">
         <v>181</v>
       </c>
-      <c r="F30" t="s">
+      <c r="H30" t="s">
+        <v>187</v>
+      </c>
+      <c r="I30" t="s">
         <v>182</v>
-      </c>
-      <c r="G30" t="s">
-        <v>183</v>
-      </c>
-      <c r="H30" t="s">
-        <v>189</v>
-      </c>
-      <c r="I30" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
@@ -1858,28 +1858,28 @@
         <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C31">
         <v>2024</v>
       </c>
       <c r="D31" t="s">
+        <v>183</v>
+      </c>
+      <c r="E31" t="s">
         <v>185</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
+        <v>186</v>
+      </c>
+      <c r="G31" t="s">
+        <v>181</v>
+      </c>
+      <c r="H31" t="s">
         <v>187</v>
       </c>
-      <c r="F31" t="s">
-        <v>188</v>
-      </c>
-      <c r="G31" t="s">
-        <v>183</v>
-      </c>
-      <c r="H31" t="s">
-        <v>189</v>
-      </c>
       <c r="I31" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
still fixing jimmy jordan's picture
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE1E8EE-4C11-4C2E-BE36-CBBEE490528F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEFA812-FA8C-4574-8C06-A34C291D3EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10" yWindow="0" windowWidth="19180" windowHeight="10080" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
@@ -615,7 +615,7 @@
     <t>Almost 100 years ago, Balto, along with a pack of elite sled dogs helped save the community of Nome, Alaska, from a diphtheria outbreak. Balto is representative of the sled dogs of the era who were reputed for their hardiness, endurance, and tolerance of harsh conditions at a time when northern communities relied on them for transportation, protection, and companionship. Unlike modern breeds, Balto and his contemporaries were products of generations of mating of diverse, outbred dogs selected for their performance and hardiness.  Today, Balto is immortalized with a statue in Central Park and is physically preserved and on display at the Cleaveland Museum of Natural History. We asked ourselves, could we use advances in genomic technologies and ancient DNA recovery techniques to parse through Balto’s DNA and understand selection emphasis and diversity occurring in sled dogs in the 1930’s? Could we decipher Balto’s physical appearance from his DNA and identify healthy developmental gene variants that may have endowed sled dogs in that era with abilities to withstand and thrive in harsh environments? Could we use our findings to guide modern breeders to breed healthier dogs? &lt;br&gt;&lt;br&gt;Also, here's a photo of Dr. Huson racing as a musher in Alaska!&lt;div class="box"&gt; &lt;img src="images/huson_sled.jpg" class='center'&gt; &lt;/div&gt;</t>
   </si>
   <si>
-    <t>The newspaper industry in the U.S. has been undergoing a significant decline since the early 2000s. The rise of the internet ushered in an era of information abundance and accessibility. However, this transition has severely impacted the traditional business models that once supported local newspapers, resulting in noticeable gaps in community coverage across the country. All of this is set against a climate where trust in media is approaching historic lows in the U.S.&lt;br&gt;&lt;br&gt;This presentation will illustrate these challenges, both on a local scale and within a broader context. Additionally, we will delve into the new models that are being explored in an effort to revitalize local reporting.&lt;br&gt;&lt;br&gt;&lt;div class="box"&gt; &lt;img src="images/Oct_4_2023_Jimmy_Jordan_1.jpg" style = 'width: 250' class='center'&gt; &lt;/div&gt;</t>
+    <t>The newspaper industry in the U.S. has been undergoing a significant decline since the early 2000s. The rise of the internet ushered in an era of information abundance and accessibility. However, this transition has severely impacted the traditional business models that once supported local newspapers, resulting in noticeable gaps in community coverage across the country. All of this is set against a climate where trust in media is approaching historic lows in the U.S.&lt;br&gt;&lt;br&gt;This presentation will illustrate these challenges, both on a local scale and within a broader context. Additionally, we will delve into the new models that are being explored in an effort to revitalize local reporting.&lt;br&gt;&lt;br&gt;&lt;div class="box"&gt; &lt;img src="images/Oct_4_2023_Jimmy_Jordan_1.jpg" style = 'width: 100' class='center'&gt; &lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -974,7 +974,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
added December photos to folder and past events page
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AED9EB-23BA-4E7D-AEB2-7890E49D2EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129D4B13-DECB-474D-849A-0C259BC5A083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10" yWindow="0" windowWidth="19180" windowHeight="10080" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
@@ -564,12 +564,6 @@
     <t>Justifying Slavery: The Intellectual Background of the Reconstruction Amendments</t>
   </si>
   <si>
-    <t xml:space="preserve"> Recent appraisals of the Thirteenth Amendment to the United States Constitution often note with alarm that slavery remains a legal form of punishment and lament for how this loophole has been weaponized against black Americans. I’m interested in how this alarm reflects an Aristotelian attitude towards slavery (more on what that means in the talk!), and about how an intellectual history of various justifications for slavery can help us understand what’s going on in the Thirteenth Amendment.</t>
-  </si>
-  <si>
-    <t>Do you find yourself freaking out over the state of the global environment, climate change, and loss of biodiversity? If so, you’re not alone — eco-anxiety has become one of the leading mental health issues in the third decade of the 21st century. Public gardens, which include botanic gardens, arboreta, conservatories, and historic landscapes, are addressing these seemingly overwhelming environmental challenges through their extensive collections, protection of natural areas, preservation of endangered species, and through programming and messaging. Will public gardens single-handedly solve all of these problems? No, but they can be a significant contributor to the solutions. In this talk you’ll learn some of the ways they are making a difference.</t>
-  </si>
-  <si>
     <t>February 7th</t>
   </si>
   <si>
@@ -616,6 +610,12 @@
   </si>
   <si>
     <t>The newspaper industry in the U.S. has been undergoing a significant decline since the early 2000s. The rise of the internet ushered in an era of information abundance and accessibility. However, this transition has severely impacted the traditional business models that once supported local newspapers, resulting in noticeable gaps in community coverage across the country. All of this is set against a climate where trust in media is approaching historic lows in the U.S.&lt;br&gt;&lt;br&gt;This presentation will illustrate these challenges, both on a local scale and within a broader context. Additionally, we will delve into the new models that are being explored in an effort to revitalize local reporting.&lt;br&gt;&lt;br&gt;&lt;div class="box"&gt; &lt;img src="images/Oct_4_2023_Jimmy_Jordan_1.jpg" style = 'width: 300' class='center'&gt; &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Do you find yourself freaking out over the state of the global environment, climate change, and loss of biodiversity? If so, you’re not alone — eco-anxiety has become one of the leading mental health issues in the third decade of the 21st century. Public gardens, which include botanic gardens, arboreta, conservatories, and historic landscapes, are addressing these seemingly overwhelming environmental challenges through their extensive collections, protection of natural areas, preservation of endangered species, and through programming and messaging. Will public gardens single-handedly solve all of these problems? No, but they can be a significant contributor to the solutions. In this talk you’ll learn some of the ways they are making a difference. &lt;br&gt;&lt;br&gt;&lt;div class="box"&gt; &lt;img src="Dec_6_2023_Donald_Rakow_1.jpg" class='center'&gt; &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Recent appraisals of the Thirteenth Amendment to the United States Constitution often note with alarm that slavery remains a legal form of punishment and lament for how this loophole has been weaponized against black Americans. I’m interested in how this alarm reflects an Aristotelian attitude towards slavery (more on what that means in the talk!), and about how an intellectual history of various justifications for slavery can help us understand what’s going on in the Thirteenth Amendment. &lt;br&gt;&lt;br&gt;&lt;div class="box"&gt; &lt;img src="Dec_6_2023_Toni_Alimi_1.jpg" class='center'&gt; &lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -974,7 +974,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1615,7 +1615,7 @@
         <v>117</v>
       </c>
       <c r="H22" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I22" t="s">
         <v>154</v>
@@ -1673,7 +1673,7 @@
         <v>127</v>
       </c>
       <c r="H24" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I24" t="s">
         <v>156</v>
@@ -1702,7 +1702,7 @@
         <v>121</v>
       </c>
       <c r="H25" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I25" t="s">
         <v>157</v>
@@ -1731,7 +1731,7 @@
         <v>161</v>
       </c>
       <c r="H26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I26" t="s">
         <v>158</v>
@@ -1760,7 +1760,7 @@
         <v>162</v>
       </c>
       <c r="H27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I27" t="s">
         <v>159</v>
@@ -1789,7 +1789,7 @@
         <v>165</v>
       </c>
       <c r="H28" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="I28" t="s">
         <v>169</v>
@@ -1818,7 +1818,7 @@
         <v>174</v>
       </c>
       <c r="H29" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="I29" t="s">
         <v>170</v>
@@ -1829,28 +1829,28 @@
         <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C30">
         <v>2024</v>
       </c>
       <c r="D30" t="s">
+        <v>176</v>
+      </c>
+      <c r="E30" t="s">
+        <v>177</v>
+      </c>
+      <c r="F30" t="s">
         <v>178</v>
       </c>
-      <c r="E30" t="s">
+      <c r="G30" t="s">
         <v>179</v>
       </c>
-      <c r="F30" t="s">
+      <c r="H30" t="s">
+        <v>185</v>
+      </c>
+      <c r="I30" t="s">
         <v>180</v>
-      </c>
-      <c r="G30" t="s">
-        <v>181</v>
-      </c>
-      <c r="H30" t="s">
-        <v>187</v>
-      </c>
-      <c r="I30" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
@@ -1858,28 +1858,28 @@
         <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C31">
         <v>2024</v>
       </c>
       <c r="D31" t="s">
+        <v>181</v>
+      </c>
+      <c r="E31" t="s">
         <v>183</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
+        <v>184</v>
+      </c>
+      <c r="G31" t="s">
+        <v>179</v>
+      </c>
+      <c r="H31" t="s">
         <v>185</v>
       </c>
-      <c r="F31" t="s">
-        <v>186</v>
-      </c>
-      <c r="G31" t="s">
-        <v>181</v>
-      </c>
-      <c r="H31" t="s">
-        <v>187</v>
-      </c>
       <c r="I31" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed typos in talk introduction lines
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBAC97A-FE22-4D5A-82A2-434D659A7E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C3DF0D-1ADE-4CF4-A939-08DD58F837D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="0" windowWidth="19180" windowHeight="10080" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
+    <workbookView xWindow="10" yWindow="0" windowWidth="19180" windowHeight="9810" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -573,9 +573,6 @@
     <t>Outreach and Information Services Librarian for the Cornell Prison Education Program</t>
   </si>
   <si>
-    <t>radical librarianship</t>
-  </si>
-  <si>
     <t>Title coming soon!</t>
   </si>
   <si>
@@ -591,9 +588,6 @@
     <t>Geoffrey S.M. Hedrick Senior Endowed Professor of Mechanical and Aerospace Engineering</t>
   </si>
   <si>
-    <t>robotics</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -616,6 +610,12 @@
   </si>
   <si>
     <t xml:space="preserve"> Recent appraisals of the Thirteenth Amendment to the United States Constitution often note with alarm that slavery remains a legal form of punishment and lament for how this loophole has been weaponized against black Americans. I’m interested in how this alarm reflects an Aristotelian attitude towards slavery (more on what that means in the talk!), and about how an intellectual history of various justifications for slavery can help us understand what’s going on in the Thirteenth Amendment. &lt;br&gt;&lt;br&gt;&lt;div class="box"&gt; &lt;img src="images/Dec_6_2023_Toni_Alimi_1.jpg" class='center'&gt; &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>a radical librarianship</t>
+  </si>
+  <si>
+    <t>a robotics</t>
   </si>
 </sst>
 </file>
@@ -973,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F859F76-284E-4154-B5CC-2AAD28AB7940}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1615,7 +1615,7 @@
         <v>117</v>
       </c>
       <c r="H22" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I22" t="s">
         <v>154</v>
@@ -1673,7 +1673,7 @@
         <v>127</v>
       </c>
       <c r="H24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I24" t="s">
         <v>156</v>
@@ -1702,7 +1702,7 @@
         <v>121</v>
       </c>
       <c r="H25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I25" t="s">
         <v>157</v>
@@ -1731,7 +1731,7 @@
         <v>161</v>
       </c>
       <c r="H26" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I26" t="s">
         <v>158</v>
@@ -1760,7 +1760,7 @@
         <v>162</v>
       </c>
       <c r="H27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I27" t="s">
         <v>159</v>
@@ -1789,7 +1789,7 @@
         <v>165</v>
       </c>
       <c r="H28" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I28" t="s">
         <v>169</v>
@@ -1818,7 +1818,7 @@
         <v>174</v>
       </c>
       <c r="H29" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I29" t="s">
         <v>170</v>
@@ -1841,16 +1841,16 @@
         <v>177</v>
       </c>
       <c r="F30" t="s">
+        <v>191</v>
+      </c>
+      <c r="G30" t="s">
         <v>178</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
+        <v>183</v>
+      </c>
+      <c r="I30" t="s">
         <v>179</v>
-      </c>
-      <c r="H30" t="s">
-        <v>185</v>
-      </c>
-      <c r="I30" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
@@ -1864,22 +1864,22 @@
         <v>2024</v>
       </c>
       <c r="D31" t="s">
+        <v>180</v>
+      </c>
+      <c r="E31" t="s">
+        <v>182</v>
+      </c>
+      <c r="F31" t="s">
+        <v>192</v>
+      </c>
+      <c r="G31" t="s">
+        <v>178</v>
+      </c>
+      <c r="H31" t="s">
+        <v>183</v>
+      </c>
+      <c r="I31" t="s">
         <v>181</v>
-      </c>
-      <c r="E31" t="s">
-        <v>183</v>
-      </c>
-      <c r="F31" t="s">
-        <v>184</v>
-      </c>
-      <c r="G31" t="s">
-        <v>179</v>
-      </c>
-      <c r="H31" t="s">
-        <v>185</v>
-      </c>
-      <c r="I31" t="s">
-        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added titles and talks for March
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C3DF0D-1ADE-4CF4-A939-08DD58F837D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32079C5-3C6A-44A1-A829-044C9AD3891D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10" yWindow="0" windowWidth="19180" windowHeight="9810" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="195">
   <si>
     <t>speaker</t>
   </si>
@@ -573,9 +572,6 @@
     <t>Outreach and Information Services Librarian for the Cornell Prison Education Program</t>
   </si>
   <si>
-    <t>Title coming soon!</t>
-  </si>
-  <si>
     <t>mreynolds</t>
   </si>
   <si>
@@ -588,9 +584,6 @@
     <t>Geoffrey S.M. Hedrick Senior Endowed Professor of Mechanical and Aerospace Engineering</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Ever wonder how others perceive you based on your actions? We all do. Shockingly, recent studies in psychology reveal we're often quite mistaken about these perceptions. For example, people think they're less liked by others than they actually are, or they assume others aren't interested in their unsolicited advice when in fact they are. Such findings could help us get along better with others. But how accurate are these studies? And is it possible that participants in these studies are just trying to appear 'nice' when answering research questions? In this talk, I'll share my own research on this topic and discuss if we should take these findings at face value. Join me to discuss the fascinating, messy world of how we're seen by others.&lt;br&gt;&lt;br&gt;&lt;div class="box"&gt; &lt;img src="images/Nov_1_2023_Andres_Montealegre_1.jpg" class='center'&gt; &lt;/div&gt;</t>
   </si>
   <si>
@@ -616,6 +609,18 @@
   </si>
   <si>
     <t>a robotics</t>
+  </si>
+  <si>
+    <t>Will Robots Kill Us?</t>
+  </si>
+  <si>
+    <t>You know the sci fi trope — humanity depends on robots that decide to kill us all until a hero shows up to stop their evil plan. How close is that to reality? Will robots take over the world? Are they dangerous? Will they be? In this talk I'll describe what robots can and cannot do these days and discuss what the future might look like.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> New York State prisons are low-information environments, where there is no internet access and books and media are subject to strict censorship. How can librarians on the outside respond to incarcerated patrons' need for books and information? The Cornell Prison Education Program (CPEP) is grappling with these questions as they seek to create research opportunities and expand information access in prison in anticipation of their launch of a Cornell BA inside. In this talk, we'll discuss what it's like to build a library program for incarcerated students, introducing Cornell's world class research materials behind the walls. We'll learn about CPEP and its history, nationwide efforts to bring library resources to incarcerated patrons, and what we're doing at Cornell to provide incarcerated students with more academic resources. We'll also talk about how to get involved in CPEP! </t>
+  </si>
+  <si>
+    <t>Bringing the Library to Prison with the Cornell Prison Education Program</t>
   </si>
 </sst>
 </file>
@@ -973,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F859F76-284E-4154-B5CC-2AAD28AB7940}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1615,7 +1620,7 @@
         <v>117</v>
       </c>
       <c r="H22" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I22" t="s">
         <v>154</v>
@@ -1673,7 +1678,7 @@
         <v>127</v>
       </c>
       <c r="H24" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I24" t="s">
         <v>156</v>
@@ -1702,7 +1707,7 @@
         <v>121</v>
       </c>
       <c r="H25" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I25" t="s">
         <v>157</v>
@@ -1731,7 +1736,7 @@
         <v>161</v>
       </c>
       <c r="H26" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I26" t="s">
         <v>158</v>
@@ -1760,7 +1765,7 @@
         <v>162</v>
       </c>
       <c r="H27" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I27" t="s">
         <v>159</v>
@@ -1789,7 +1794,7 @@
         <v>165</v>
       </c>
       <c r="H28" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I28" t="s">
         <v>169</v>
@@ -1818,7 +1823,7 @@
         <v>174</v>
       </c>
       <c r="H29" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I29" t="s">
         <v>170</v>
@@ -1841,19 +1846,19 @@
         <v>177</v>
       </c>
       <c r="F30" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G30" t="s">
+        <v>194</v>
+      </c>
+      <c r="H30" t="s">
+        <v>193</v>
+      </c>
+      <c r="I30" t="s">
         <v>178</v>
       </c>
-      <c r="H30" t="s">
-        <v>183</v>
-      </c>
-      <c r="I30" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>15</v>
       </c>
@@ -1864,22 +1869,22 @@
         <v>2024</v>
       </c>
       <c r="D31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E31" t="s">
+        <v>181</v>
+      </c>
+      <c r="F31" t="s">
+        <v>190</v>
+      </c>
+      <c r="G31" t="s">
+        <v>191</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="I31" t="s">
         <v>180</v>
-      </c>
-      <c r="E31" t="s">
-        <v>182</v>
-      </c>
-      <c r="F31" t="s">
-        <v>192</v>
-      </c>
-      <c r="G31" t="s">
-        <v>178</v>
-      </c>
-      <c r="H31" t="s">
-        <v>183</v>
-      </c>
-      <c r="I31" t="s">
-        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Elias' abstract and title
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDDF6A9-57C4-4909-88B6-E1D9CD8C4E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A156A632-1B84-403F-BCA4-9828DEB64319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="0" windowWidth="19180" windowHeight="9810" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -650,13 +650,16 @@
     <t>PhD Candidate in Comparative Literature at Cornell University</t>
   </si>
   <si>
-    <t>Title Coming Soon!</t>
-  </si>
-  <si>
     <t>ebeltran</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>Latinidad Sinofonica: Asian Diasporic Visibilities in Salsa and Reggaetón</t>
+  </si>
+  <si>
+    <t>Salsa music and reggaetón, though most clearly articulated in the Hispanophone Caribbean, are related by diasporic connections coming from “histories of migrations and
+cultural exchange throughout all of the Americas.” And, though some scholars suggest that reggaetón should be read through its social and political “positioning to cultural expressions exclusively centered on blackness,” I respectfully disagree. While holding—and celebrating(!)—the African Diaspora as a creative nexus in both genres, exclusively positioning the cultural expressions of either salsa or reggaetón on blackness keeps us from connecting “asymmetrical histories and processes” that have, all too often, been examined separately, rather than approached as responses to shared conditions with deep implications. Looking at the musical presences and relations between African and Asian Diasporic subjects in salsa and reggateón refuses not only the idea of separate histories, but also exposes how racialized
+mimicry fuels antagonisms, and reinforces colonial subjects as negatively known and dispositively knowable. In this way, looking at the presence and contributions of the Chinese
+Diaspora in the musics of the Hispanophone Caribbean, previously a site of occlusion, emerges not as a pitting against but as a potential source of coalition-building precisely because of the intimacy of shared histories.</t>
   </si>
 </sst>
 </file>
@@ -1014,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F859F76-284E-4154-B5CC-2AAD28AB7940}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="C33" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1952,7 +1955,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>16</v>
       </c>
@@ -1972,13 +1975,13 @@
         <v>61</v>
       </c>
       <c r="G33" t="s">
+        <v>205</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="I33" t="s">
         <v>204</v>
-      </c>
-      <c r="H33" t="s">
-        <v>206</v>
-      </c>
-      <c r="I33" t="s">
-        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added February photos to website
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A0403B-55C2-458B-B46E-E68E727A14B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BBBCE7-D841-4587-9ABD-3208FDF40EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -614,12 +614,6 @@
     <t>Will Robots Kill Us?</t>
   </si>
   <si>
-    <t>You know the sci fi trope — humanity depends on robots that decide to kill us all until a hero shows up to stop their evil plan. How close is that to reality? Will robots take over the world? Are they dangerous? Will they be? In this talk I'll describe what robots can and cannot do these days and discuss what the future might look like.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> New York State prisons are low-information environments, where there is no internet access and books and media are subject to strict censorship. How can librarians on the outside respond to incarcerated patrons' need for books and information? The Cornell Prison Education Program (CPEP) is grappling with these questions as they seek to create research opportunities and expand information access in prison in anticipation of their launch of a Cornell BA inside. In this talk, we'll discuss what it's like to build a library program for incarcerated students, introducing Cornell's world class research materials behind the walls. We'll learn about CPEP and its history, nationwide efforts to bring library resources to incarcerated patrons, and what we're doing at Cornell to provide incarcerated students with more academic resources. We'll also talk about how to get involved in CPEP! </t>
-  </si>
-  <si>
     <t>Bringing the Library to Prison with the Cornell Prison Education Program</t>
   </si>
   <si>
@@ -658,6 +652,12 @@
   <si>
     <t>Salsa music and reggaetón, though most clearly articulated in the Hispanophone Caribbean, are related by diasporic connections coming from “histories of migrations and cultural exchange throughout all of the Americas.” And, though some scholars suggest that reggaetón should be read through its social and political “positioning to cultural expressions exclusively centered on blackness,” I respectfully disagree. While holding—and celebrating(!)—the African Diaspora as a creative nexus in both genres, exclusively positioning the cultural expressions of either salsa or reggaetón on blackness keeps us from connecting “asymmetrical histories and processes” that have, all too often, been examined separately, rather than approached as responses to shared conditions with deep implications. Looking at the musical presences and relations between African and Asian Diasporic subjects in salsa and reggateón refuses not only the idea of separate histories, but also exposes how racialized
 mimicry fuels antagonisms, and reinforces colonial subjects as negatively known and dispositively knowable. In this way, looking at the presence and contributions of the Chinese Diaspora in the musics of the Hispanophone Caribbean, previously a site of occlusion, emerges not as a pitting against but as a potential source of coalition-building precisely because of the intimacy of shared histories.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> New York State prisons are low-information environments, where there is no internet access and books and media are subject to strict censorship. How can librarians on the outside respond to incarcerated patrons' need for books and information? The Cornell Prison Education Program (CPEP) is grappling with these questions as they seek to create research opportunities and expand information access in prison in anticipation of their launch of a Cornell BA inside. In this talk, we'll discuss what it's like to build a library program for incarcerated students, introducing Cornell's world class research materials behind the walls. We'll learn about CPEP and its history, nationwide efforts to bring library resources to incarcerated patrons, and what we're doing at Cornell to provide incarcerated students with more academic resources. We'll also talk about how to get involved in CPEP! &lt;br&gt;&lt;br&gt;&lt;div class="box"&gt; &lt;img src="images/Feb 7_ 2024_Maddie_Reynolds_1" class='center'&gt; &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>You know the sci fi trope — humanity depends on robots that decide to kill us all until a hero shows up to stop their evil plan. How close is that to reality? Will robots take over the world? Are they dangerous? Will they be? In this talk I'll describe what robots can and cannot do these days and discuss what the future might look like.&lt;img src="images/Feb 7_ 2024_Hadas_Kress-Gazit_1" class='center'&gt; &lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -717,9 +717,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -757,7 +757,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -863,7 +863,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1005,7 +1005,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1015,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F859F76-284E-4154-B5CC-2AAD28AB7940}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C33" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1886,10 +1886,10 @@
         <v>189</v>
       </c>
       <c r="G30" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H30" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="I30" t="s">
         <v>178</v>
@@ -1918,7 +1918,7 @@
         <v>191</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="I31" t="s">
         <v>180</v>
@@ -1929,57 +1929,57 @@
         <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C32">
         <v>2024</v>
       </c>
       <c r="D32" t="s">
+        <v>194</v>
+      </c>
+      <c r="E32" t="s">
+        <v>195</v>
+      </c>
+      <c r="F32" t="s">
         <v>196</v>
       </c>
-      <c r="E32" t="s">
+      <c r="G32" t="s">
         <v>197</v>
       </c>
-      <c r="F32" t="s">
+      <c r="H32" t="s">
         <v>198</v>
       </c>
-      <c r="G32" t="s">
+      <c r="I32" t="s">
         <v>199</v>
       </c>
-      <c r="H32" t="s">
-        <v>200</v>
-      </c>
-      <c r="I32" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C33">
         <v>2024</v>
       </c>
       <c r="D33" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E33" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F33" t="s">
         <v>61</v>
       </c>
       <c r="G33" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I33" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed February photo typo
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BBBCE7-D841-4587-9ABD-3208FDF40EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D92102-2D4D-453D-BC8F-F39DD23ADE78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
@@ -654,10 +654,10 @@
 mimicry fuels antagonisms, and reinforces colonial subjects as negatively known and dispositively knowable. In this way, looking at the presence and contributions of the Chinese Diaspora in the musics of the Hispanophone Caribbean, previously a site of occlusion, emerges not as a pitting against but as a potential source of coalition-building precisely because of the intimacy of shared histories.</t>
   </si>
   <si>
-    <t xml:space="preserve"> New York State prisons are low-information environments, where there is no internet access and books and media are subject to strict censorship. How can librarians on the outside respond to incarcerated patrons' need for books and information? The Cornell Prison Education Program (CPEP) is grappling with these questions as they seek to create research opportunities and expand information access in prison in anticipation of their launch of a Cornell BA inside. In this talk, we'll discuss what it's like to build a library program for incarcerated students, introducing Cornell's world class research materials behind the walls. We'll learn about CPEP and its history, nationwide efforts to bring library resources to incarcerated patrons, and what we're doing at Cornell to provide incarcerated students with more academic resources. We'll also talk about how to get involved in CPEP! &lt;br&gt;&lt;br&gt;&lt;div class="box"&gt; &lt;img src="images/Feb 7_ 2024_Maddie_Reynolds_1" class='center'&gt; &lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>You know the sci fi trope — humanity depends on robots that decide to kill us all until a hero shows up to stop their evil plan. How close is that to reality? Will robots take over the world? Are they dangerous? Will they be? In this talk I'll describe what robots can and cannot do these days and discuss what the future might look like.&lt;img src="images/Feb 7_ 2024_Hadas_Kress-Gazit_1" class='center'&gt; &lt;/div&gt;</t>
+    <t>You know the sci fi trope — humanity depends on robots that decide to kill us all until a hero shows up to stop their evil plan. How close is that to reality? Will robots take over the world? Are they dangerous? Will they be? In this talk I'll describe what robots can and cannot do these days and discuss what the future might look like.&lt;img src="images/Feb 7_ 2024_Hadas_Kress-Gazit_1.jpg" class='center'&gt; &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> New York State prisons are low-information environments, where there is no internet access and books and media are subject to strict censorship. How can librarians on the outside respond to incarcerated patrons' need for books and information? The Cornell Prison Education Program (CPEP) is grappling with these questions as they seek to create research opportunities and expand information access in prison in anticipation of their launch of a Cornell BA inside. In this talk, we'll discuss what it's like to build a library program for incarcerated students, introducing Cornell's world class research materials behind the walls. We'll learn about CPEP and its history, nationwide efforts to bring library resources to incarcerated patrons, and what we're doing at Cornell to provide incarcerated students with more academic resources. We'll also talk about how to get involved in CPEP! &lt;br&gt;&lt;br&gt;&lt;div class="box"&gt; &lt;img src="images/Feb 7_ 2024_Maddie_Reynolds_1.jpg" class='center'&gt; &lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1016,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1889,7 +1889,7 @@
         <v>192</v>
       </c>
       <c r="H30" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="I30" t="s">
         <v>178</v>
@@ -1918,7 +1918,7 @@
         <v>191</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I31" t="s">
         <v>180</v>

</xml_diff>

<commit_message>
added April speakers for real
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C2EDE9-7E47-4B70-B720-D3E842B50F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA13C89B-B5D0-461A-8822-E728C13F9A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
@@ -1073,7 +1073,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
added science speaker May
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AD51FF-214C-4177-9CE1-D5AC0C5FBB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4831FA8A-3A2E-439E-AACF-31C04685970F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
@@ -706,12 +706,6 @@
     <t>Accelerator Physicist at CLASSE</t>
   </si>
   <si>
-    <t>Title Coming Soon!</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>achapelain</t>
   </si>
   <si>
@@ -728,6 +722,13 @@
   </si>
   <si>
     <t>khaines-eitzen</t>
+  </si>
+  <si>
+    <t>Particles? Accelerators? Wait, Why Should I Care?': The Societal Benefits of Fundamental Science</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Particle and accelerator physics might sound like science fiction to you, but they affect us in the real world more than you might think (in a good way!). Let’s dive into these fields of research and see what they are, where they come from, and how they have changed our everyday lives. We’ll start with a brief overview and history before getting into some applications.
+</t>
   </si>
 </sst>
 </file>
@@ -1094,8 +1095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F859F76-284E-4154-B5CC-2AAD28AB7940}">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="G40" sqref="G37:G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2133,22 +2134,22 @@
         <v>220</v>
       </c>
       <c r="E36" t="s">
+        <v>223</v>
+      </c>
+      <c r="F36" t="s">
+        <v>224</v>
+      </c>
+      <c r="G36" t="s">
         <v>225</v>
       </c>
-      <c r="F36" t="s">
+      <c r="H36" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="G36" t="s">
+      <c r="I36" t="s">
         <v>227</v>
       </c>
-      <c r="H36" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="I36" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>18</v>
       </c>
@@ -2167,14 +2168,14 @@
       <c r="F37" t="s">
         <v>55</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="I37" t="s">
         <v>222</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="I37" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
reworded September political talk
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C74DF8-8523-482F-BEEE-060FFF7B9B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AAB901-B1AA-4686-8502-1E86C3703F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
@@ -883,9 +883,6 @@
     <t>Members of the TeenDay Ithaca Model United Nations Team</t>
   </si>
   <si>
-    <t>a political debate</t>
-  </si>
-  <si>
     <t>Dr. Elizabeth Medina-Gray</t>
   </si>
   <si>
@@ -905,6 +902,9 @@
   </si>
   <si>
     <t>a musicology</t>
+  </si>
+  <si>
+    <t>a political dialogue</t>
   </si>
 </sst>
 </file>
@@ -1281,8 +1281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F859F76-284E-4154-B5CC-2AAD28AB7940}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2549,22 +2549,22 @@
         <v>2024</v>
       </c>
       <c r="D44" t="s">
+        <v>273</v>
+      </c>
+      <c r="E44" t="s">
         <v>274</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
+        <v>279</v>
+      </c>
+      <c r="G44" t="s">
+        <v>276</v>
+      </c>
+      <c r="H44" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="F44" t="s">
-        <v>280</v>
-      </c>
-      <c r="G44" t="s">
+      <c r="I44" t="s">
         <v>277</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="I44" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
@@ -2584,7 +2584,7 @@
         <v>272</v>
       </c>
       <c r="F45" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="G45" t="s">
         <v>269</v>
@@ -2593,7 +2593,7 @@
         <v>270</v>
       </c>
       <c r="I45" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed October speakers hopefully
</commit_message>
<xml_diff>
--- a/generator/public works.xlsx
+++ b/generator/public works.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lfrancis\ithacapublicworks.github.io\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D045A3CF-1FC4-4810-8C87-94E154B2AF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884E404A-D4AB-4E17-B403-6847D9B93EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E1829570-05EC-4F9A-A973-1191B70B70D1}"/>
   </bookViews>
@@ -910,42 +910,40 @@
     <t>Earth Source Heat: Digging Deep for Climate Solutions</t>
   </si>
   <si>
-    <t xml:space="preserve">We know we need to get off fossil fuels, but how do you do it if you are a 30,000-person research university? Cornell is investigating Deep Direct Use Geothermal Energy as a possible path to meeting carbon free campus heating needs. If you go deep enough (10,000’ below the surface), the heat is there – but how to get it?
-</t>
-  </si>
-  <si>
     <t>Wayne Bezner Kerr</t>
   </si>
   <si>
     <t>Cornell Earth Source Heat Program Manager</t>
   </si>
   <si>
+    <t>Pete Miller</t>
+  </si>
+  <si>
+    <t>an environmental technologies</t>
+  </si>
+  <si>
+    <t>a social philosophy</t>
+  </si>
+  <si>
+    <t>As human beings, we live in three kinds of reality. The single physical reality we all share full of rocks, trees, and beautiful gorges to walk through and appreciate them is objective. The internal mental reality we each have in our own mind made of things we remember, believe, and imagine is subjective. The social realities we share with different groups of people that are made out of things we agree about are intersubjective. These social realities influence our behavior and how we feel about life all the time, but we are rarely explicit about their nature. It took me till I was 54 to even learn the term intersubjectivity existed, and I’ve been a social philosophy nerd all my life. This talk is intended to expose the concept of intersubjectivity more fully in the hope that dragging it in to the light will give people who hear the talk a fresh and interesting perspective on how we build and update the social arrangements within which we live.</t>
+  </si>
+  <si>
+    <t>pmiller</t>
+  </si>
+  <si>
+    <t>October 3rd</t>
+  </si>
+  <si>
+    <t>Local Expert</t>
+  </si>
+  <si>
+    <t>We know we need to get off fossil fuels, but how do you do it if you are a 30,000-person research university? Cornell is investigating Deep Direct Use Geothermal Energy as a possible path to meeting carbon free campus heating needs. If you go deep enough (10,000’ below the surface), the heat is there – but how to get it?</t>
+  </si>
+  <si>
     <t>wbezner-kerr</t>
   </si>
   <si>
-    <t>Pete Miller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intersubjectivity / Constructing and Reconstructing Social Constructs
-</t>
-  </si>
-  <si>
-    <t>an environmental technologies</t>
-  </si>
-  <si>
-    <t>a social philosophy</t>
-  </si>
-  <si>
-    <t>As human beings, we live in three kinds of reality. The single physical reality we all share full of rocks, trees, and beautiful gorges to walk through and appreciate them is objective. The internal mental reality we each have in our own mind made of things we remember, believe, and imagine is subjective. The social realities we share with different groups of people that are made out of things we agree about are intersubjective. These social realities influence our behavior and how we feel about life all the time, but we are rarely explicit about their nature. It took me till I was 54 to even learn the term intersubjectivity existed, and I’ve been a social philosophy nerd all my life. This talk is intended to expose the concept of intersubjectivity more fully in the hope that dragging it in to the light will give people who hear the talk a fresh and interesting perspective on how we build and update the social arrangements within which we live.</t>
-  </si>
-  <si>
-    <t>pmiller</t>
-  </si>
-  <si>
-    <t>October 3rd</t>
-  </si>
-  <si>
-    <t>Professor of Engineering</t>
+    <t>Intersubjectivity / Constructing and Reconstructing Social Constructs</t>
   </si>
 </sst>
 </file>
@@ -1320,10 +1318,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F859F76-284E-4154-B5CC-2AAD28AB7940}">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2637,64 +2635,65 @@
         <v>278</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>23</v>
       </c>
       <c r="B46" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C46">
         <v>2024</v>
       </c>
       <c r="D46" t="s">
+        <v>282</v>
+      </c>
+      <c r="E46" t="s">
         <v>283</v>
       </c>
-      <c r="E46" t="s">
-        <v>284</v>
-      </c>
       <c r="F46" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="G46" t="s">
         <v>281</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
       <c r="I46" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>23</v>
       </c>
       <c r="B47" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C47">
         <v>2024</v>
       </c>
       <c r="D47" t="s">
+        <v>284</v>
+      </c>
+      <c r="E47" t="s">
+        <v>290</v>
+      </c>
+      <c r="F47" t="s">
         <v>286</v>
       </c>
-      <c r="E47" t="s">
+      <c r="G47" t="s">
         <v>293</v>
       </c>
-      <c r="F47" t="s">
-        <v>289</v>
-      </c>
-      <c r="G47" s="2" t="s">
+      <c r="H47" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="H47" s="2" t="s">
-        <v>290</v>
-      </c>
       <c r="I47" t="s">
-        <v>291</v>
-      </c>
-    </row>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>